<commit_message>
[Fix]#79 fix viewModel array error
</commit_message>
<xml_diff>
--- a/Projects/App/Resources/onboardingArtist.xlsx
+++ b/Projects/App/Resources/onboardingArtist.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choihyowon/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choihyowon/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415D2787-8822-3140-B59B-5704BB5E3D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E06DF69-3658-3E43-98D2-DEF01C49C229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15640" xr2:uid="{DDFC3EF1-0C9B-2449-839F-441E442BC4BA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{DDFC3EF1-0C9B-2449-839F-441E442BC4BA}"/>
   </bookViews>
   <sheets>
     <sheet name="통합(최종본)" sheetId="7" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'통합(최종본)'!$A$1:$C$261</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'통합(최종본)'!$A$1:$C$262</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="469">
   <si>
     <t>투모로우바이투게더</t>
   </si>
@@ -382,6 +382,12 @@
   </si>
   <si>
     <t xml:space="preserve">e119e5ff-0de0-421c-a630-0516c6acede8 </t>
+  </si>
+  <si>
+    <t>티아라</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4103d05e-da2a-4744-81ae-f8dc3e81728c </t>
   </si>
   <si>
     <t>H1-KEY</t>
@@ -1888,10 +1894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF8B4FB7-ABFA-AA47-A964-F8732D4F461D}">
-  <dimension ref="A1:C263"/>
+  <dimension ref="A1:C264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="164" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:C53"/>
+    <sheetView tabSelected="1" zoomScale="164" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B225" sqref="B225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="17.25" customHeight="1"/>
@@ -2521,7 +2527,7 @@
       <c r="A57" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="4" t="s">
         <v>122</v>
       </c>
       <c r="C57" s="1" t="s">
@@ -2532,7 +2538,7 @@
       <c r="A58" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -2632,7 +2638,7 @@
         <v>141</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>2</v>
@@ -2640,10 +2646,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B68" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>140</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>2</v>
@@ -2651,10 +2657,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>2</v>
@@ -2697,22 +2703,22 @@
       <c r="A73" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" s="4" t="s">
         <v>152</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>153</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="C74" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2734,7 +2740,7 @@
         <v>159</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>153</v>
+        <v>59</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2745,7 +2751,7 @@
         <v>161</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2756,7 +2762,7 @@
         <v>163</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2767,7 +2773,7 @@
         <v>165</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2778,18 +2784,18 @@
         <v>167</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>168</v>
+        <v>59</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="C81" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2800,10 +2806,10 @@
         <v>172</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" s="1" customFormat="1">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
       <c r="A83" s="1" t="s">
         <v>173</v>
       </c>
@@ -2811,7 +2817,7 @@
         <v>174</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>153</v>
+        <v>59</v>
       </c>
     </row>
     <row r="84" spans="1:3" s="1" customFormat="1">
@@ -2822,7 +2828,7 @@
         <v>176</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
     <row r="85" spans="1:3" s="1" customFormat="1">
@@ -2833,7 +2839,7 @@
         <v>178</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="86" spans="1:3" s="1" customFormat="1">
@@ -2844,7 +2850,7 @@
         <v>180</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>59</v>
+        <v>170</v>
       </c>
     </row>
     <row r="87" spans="1:3" s="1" customFormat="1">
@@ -2866,18 +2872,18 @@
         <v>184</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>185</v>
+        <v>59</v>
       </c>
     </row>
     <row r="89" spans="1:3" s="1" customFormat="1">
       <c r="A89" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="C89" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="90" spans="1:3" s="1" customFormat="1">
@@ -2888,7 +2894,7 @@
         <v>189</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="91" spans="1:3" s="1" customFormat="1">
@@ -2899,7 +2905,7 @@
         <v>191</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>153</v>
+        <v>59</v>
       </c>
     </row>
     <row r="92" spans="1:3" s="1" customFormat="1">
@@ -2910,7 +2916,7 @@
         <v>193</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="93" spans="1:3" s="1" customFormat="1">
@@ -2954,7 +2960,7 @@
         <v>201</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>185</v>
+        <v>59</v>
       </c>
     </row>
     <row r="97" spans="1:3" s="1" customFormat="1">
@@ -2965,7 +2971,7 @@
         <v>203</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>59</v>
+        <v>187</v>
       </c>
     </row>
     <row r="98" spans="1:3" s="1" customFormat="1">
@@ -3009,7 +3015,7 @@
         <v>211</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>153</v>
+        <v>59</v>
       </c>
     </row>
     <row r="102" spans="1:3" s="1" customFormat="1">
@@ -3020,7 +3026,7 @@
         <v>213</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="103" spans="1:3" s="1" customFormat="1">
@@ -3031,7 +3037,7 @@
         <v>215</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
     </row>
     <row r="104" spans="1:3" s="1" customFormat="1">
@@ -3042,7 +3048,7 @@
         <v>217</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="105" spans="1:3" s="1" customFormat="1">
@@ -3053,7 +3059,7 @@
         <v>219</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>153</v>
+        <v>187</v>
       </c>
     </row>
     <row r="106" spans="1:3" s="1" customFormat="1">
@@ -3064,7 +3070,7 @@
         <v>221</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="107" spans="1:3" s="1" customFormat="1">
@@ -3075,7 +3081,7 @@
         <v>223</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="108" spans="1:3" s="1" customFormat="1">
@@ -3108,7 +3114,7 @@
         <v>229</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>185</v>
+        <v>59</v>
       </c>
     </row>
     <row r="111" spans="1:3" s="1" customFormat="1">
@@ -3119,7 +3125,7 @@
         <v>231</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="112" spans="1:3" s="1" customFormat="1">
@@ -3130,7 +3136,7 @@
         <v>233</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="113" spans="1:3" s="1" customFormat="1">
@@ -3141,7 +3147,7 @@
         <v>235</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="114" spans="1:3" s="1" customFormat="1">
@@ -3152,7 +3158,7 @@
         <v>237</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="115" spans="1:3" s="1" customFormat="1">
@@ -3163,7 +3169,7 @@
         <v>239</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="116" spans="1:3" s="1" customFormat="1">
@@ -3174,7 +3180,7 @@
         <v>241</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="117" spans="1:3" s="1" customFormat="1">
@@ -3185,7 +3191,7 @@
         <v>243</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>153</v>
+        <v>187</v>
       </c>
     </row>
     <row r="118" spans="1:3" s="1" customFormat="1">
@@ -3196,7 +3202,7 @@
         <v>245</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="119" spans="1:3" s="1" customFormat="1">
@@ -3229,7 +3235,7 @@
         <v>251</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>168</v>
+        <v>59</v>
       </c>
     </row>
     <row r="122" spans="1:3" s="1" customFormat="1">
@@ -3239,19 +3245,19 @@
       <c r="B122" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C122" s="3" t="s">
-        <v>254</v>
+      <c r="C122" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="123" spans="1:3" s="1" customFormat="1">
       <c r="A123" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B123" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="C123" s="3" t="s">
         <v>256</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:3" s="1" customFormat="1">
@@ -3262,7 +3268,7 @@
         <v>258</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>185</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:3" s="1" customFormat="1">
@@ -3273,7 +3279,7 @@
         <v>260</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>168</v>
+        <v>187</v>
       </c>
     </row>
     <row r="126" spans="1:3" s="1" customFormat="1">
@@ -3284,7 +3290,7 @@
         <v>262</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>153</v>
+        <v>170</v>
       </c>
     </row>
     <row r="127" spans="1:3" s="1" customFormat="1">
@@ -3295,7 +3301,7 @@
         <v>264</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="128" spans="1:3" s="1" customFormat="1">
@@ -3306,7 +3312,7 @@
         <v>266</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>185</v>
+        <v>59</v>
       </c>
     </row>
     <row r="129" spans="1:3" s="1" customFormat="1">
@@ -3317,7 +3323,7 @@
         <v>268</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="130" spans="1:3" s="1" customFormat="1">
@@ -3328,7 +3334,7 @@
         <v>270</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>153</v>
+        <v>187</v>
       </c>
     </row>
     <row r="131" spans="1:3" s="1" customFormat="1">
@@ -3339,7 +3345,7 @@
         <v>272</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="132" spans="1:3" s="1" customFormat="1">
@@ -3350,7 +3356,7 @@
         <v>274</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>185</v>
+        <v>59</v>
       </c>
     </row>
     <row r="133" spans="1:3" s="1" customFormat="1">
@@ -3361,7 +3367,7 @@
         <v>276</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="134" spans="1:3" s="1" customFormat="1">
@@ -3372,7 +3378,7 @@
         <v>278</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="135" spans="1:3" s="1" customFormat="1">
@@ -3383,7 +3389,7 @@
         <v>280</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="136" spans="1:3" s="1" customFormat="1">
@@ -3394,7 +3400,7 @@
         <v>282</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="137" spans="1:3" s="1" customFormat="1">
@@ -3405,7 +3411,7 @@
         <v>284</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>59</v>
+        <v>187</v>
       </c>
     </row>
     <row r="138" spans="1:3" s="1" customFormat="1">
@@ -3416,7 +3422,7 @@
         <v>286</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>185</v>
+        <v>59</v>
       </c>
     </row>
     <row r="139" spans="1:3" s="1" customFormat="1">
@@ -3427,7 +3433,7 @@
         <v>288</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>153</v>
+        <v>187</v>
       </c>
     </row>
     <row r="140" spans="1:3" s="1" customFormat="1">
@@ -3438,7 +3444,7 @@
         <v>290</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
     </row>
     <row r="141" spans="1:3" s="1" customFormat="1">
@@ -3449,7 +3455,7 @@
         <v>292</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>168</v>
+        <v>187</v>
       </c>
     </row>
     <row r="142" spans="1:3" s="1" customFormat="1">
@@ -3460,7 +3466,7 @@
         <v>294</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="143" spans="1:3" s="1" customFormat="1">
@@ -3471,7 +3477,7 @@
         <v>296</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="144" spans="1:3" s="1" customFormat="1">
@@ -3482,7 +3488,7 @@
         <v>298</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="145" spans="1:3" s="1" customFormat="1">
@@ -3493,7 +3499,7 @@
         <v>300</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="146" spans="1:3" s="1" customFormat="1">
@@ -3504,7 +3510,7 @@
         <v>302</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>153</v>
+        <v>170</v>
       </c>
     </row>
     <row r="147" spans="1:3" s="1" customFormat="1">
@@ -3515,7 +3521,7 @@
         <v>304</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="148" spans="1:3" s="1" customFormat="1">
@@ -3526,7 +3532,7 @@
         <v>306</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>254</v>
+        <v>59</v>
       </c>
     </row>
     <row r="149" spans="1:3" s="1" customFormat="1">
@@ -3537,7 +3543,7 @@
         <v>308</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>185</v>
+        <v>256</v>
       </c>
     </row>
     <row r="150" spans="1:3" s="1" customFormat="1">
@@ -3548,7 +3554,7 @@
         <v>310</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>153</v>
+        <v>187</v>
       </c>
     </row>
     <row r="151" spans="1:3" s="1" customFormat="1">
@@ -3559,7 +3565,7 @@
         <v>312</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="152" spans="1:3" s="1" customFormat="1">
@@ -3570,7 +3576,7 @@
         <v>314</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="153" spans="1:3" s="1" customFormat="1">
@@ -3581,7 +3587,7 @@
         <v>316</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="154" spans="1:3" s="1" customFormat="1">
@@ -3592,7 +3598,7 @@
         <v>318</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="155" spans="1:3" s="1" customFormat="1">
@@ -3603,7 +3609,7 @@
         <v>320</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
     <row r="156" spans="1:3" s="1" customFormat="1">
@@ -3614,7 +3620,7 @@
         <v>322</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>153</v>
+        <v>170</v>
       </c>
     </row>
     <row r="157" spans="1:3" s="1" customFormat="1">
@@ -3625,7 +3631,7 @@
         <v>324</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
     </row>
     <row r="158" spans="1:3" s="1" customFormat="1">
@@ -3636,7 +3642,7 @@
         <v>326</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="159" spans="1:3" s="1" customFormat="1">
@@ -3647,7 +3653,7 @@
         <v>328</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="160" spans="1:3" s="1" customFormat="1">
@@ -3658,29 +3664,29 @@
         <v>330</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>59</v>
+        <v>187</v>
       </c>
     </row>
     <row r="161" spans="1:3" s="1" customFormat="1">
-      <c r="A161" s="3" t="s">
+      <c r="A161" s="1" t="s">
         <v>331</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>332</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>185</v>
+        <v>59</v>
       </c>
     </row>
     <row r="162" spans="1:3" s="1" customFormat="1">
-      <c r="A162" s="1" t="s">
+      <c r="A162" s="3" t="s">
         <v>333</v>
       </c>
       <c r="B162" s="2" t="s">
         <v>334</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="163" spans="1:3" s="1" customFormat="1">
@@ -3691,7 +3697,7 @@
         <v>336</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="164" spans="1:3" s="1" customFormat="1">
@@ -3702,7 +3708,7 @@
         <v>338</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>153</v>
+        <v>187</v>
       </c>
     </row>
     <row r="165" spans="1:3" s="1" customFormat="1">
@@ -3713,7 +3719,7 @@
         <v>340</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="166" spans="1:3" s="1" customFormat="1">
@@ -3724,7 +3730,7 @@
         <v>342</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
     <row r="167" spans="1:3" s="1" customFormat="1">
@@ -3735,7 +3741,7 @@
         <v>344</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>153</v>
+        <v>170</v>
       </c>
     </row>
     <row r="168" spans="1:3" s="1" customFormat="1">
@@ -3746,7 +3752,7 @@
         <v>346</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="169" spans="1:3" s="1" customFormat="1">
@@ -3757,7 +3763,7 @@
         <v>348</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>185</v>
+        <v>59</v>
       </c>
     </row>
     <row r="170" spans="1:3" s="1" customFormat="1">
@@ -3768,18 +3774,18 @@
         <v>350</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>351</v>
+        <v>187</v>
       </c>
     </row>
     <row r="171" spans="1:3" s="1" customFormat="1">
       <c r="A171" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B171" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="B171" s="2" t="s">
+      <c r="C171" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="172" spans="1:3" s="1" customFormat="1">
@@ -3790,7 +3796,7 @@
         <v>355</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="173" spans="1:3" s="1" customFormat="1">
@@ -3801,7 +3807,7 @@
         <v>357</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="174" spans="1:3" s="1" customFormat="1">
@@ -3812,7 +3818,7 @@
         <v>359</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="175" spans="1:3" s="1" customFormat="1">
@@ -3823,7 +3829,7 @@
         <v>361</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="176" spans="1:3" s="1" customFormat="1">
@@ -3834,7 +3840,7 @@
         <v>363</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="177" spans="1:3" s="1" customFormat="1">
@@ -3845,7 +3851,7 @@
         <v>365</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="178" spans="1:3" s="1" customFormat="1">
@@ -3856,7 +3862,7 @@
         <v>367</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="179" spans="1:3" s="1" customFormat="1">
@@ -3867,7 +3873,7 @@
         <v>369</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="180" spans="1:3" s="1" customFormat="1">
@@ -3878,18 +3884,18 @@
         <v>371</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="181" spans="1:3" s="1" customFormat="1">
       <c r="A181" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="B181" s="4" t="s">
+      <c r="B181" s="2" t="s">
         <v>373</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="182" spans="1:3" s="1" customFormat="1">
@@ -3900,7 +3906,7 @@
         <v>375</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="183" spans="1:3" s="1" customFormat="1">
@@ -3911,7 +3917,7 @@
         <v>377</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="184" spans="1:3" s="1" customFormat="1">
@@ -3922,7 +3928,7 @@
         <v>379</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="185" spans="1:3" s="1" customFormat="1">
@@ -3933,7 +3939,7 @@
         <v>381</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="186" spans="1:3" s="1" customFormat="1">
@@ -3944,7 +3950,7 @@
         <v>383</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="187" spans="1:3" s="1" customFormat="1">
@@ -3955,7 +3961,7 @@
         <v>385</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="188" spans="1:3" s="1" customFormat="1">
@@ -3966,7 +3972,7 @@
         <v>387</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="189" spans="1:3" s="1" customFormat="1">
@@ -3977,7 +3983,7 @@
         <v>389</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="190" spans="1:3" s="1" customFormat="1">
@@ -3988,7 +3994,7 @@
         <v>391</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="191" spans="1:3" s="1" customFormat="1">
@@ -3999,7 +4005,7 @@
         <v>393</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="192" spans="1:3" s="1" customFormat="1">
@@ -4010,7 +4016,7 @@
         <v>395</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="193" spans="1:3" s="1" customFormat="1">
@@ -4021,7 +4027,7 @@
         <v>397</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="194" spans="1:3" s="1" customFormat="1">
@@ -4032,18 +4038,18 @@
         <v>399</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>400</v>
+        <v>353</v>
       </c>
     </row>
     <row r="195" spans="1:3" s="1" customFormat="1">
       <c r="A195" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B195" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="B195" s="4" t="s">
+      <c r="C195" s="1" t="s">
         <v>402</v>
-      </c>
-      <c r="C195" s="1" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="196" spans="1:3" s="1" customFormat="1">
@@ -4054,7 +4060,7 @@
         <v>404</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="197" spans="1:3" s="1" customFormat="1">
@@ -4065,7 +4071,7 @@
         <v>406</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>400</v>
+        <v>353</v>
       </c>
     </row>
     <row r="198" spans="1:3" s="1" customFormat="1">
@@ -4076,7 +4082,7 @@
         <v>408</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>351</v>
+        <v>402</v>
       </c>
     </row>
     <row r="199" spans="1:3" s="1" customFormat="1">
@@ -4087,7 +4093,7 @@
         <v>410</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>400</v>
+        <v>353</v>
       </c>
     </row>
     <row r="200" spans="1:3" s="1" customFormat="1">
@@ -4098,18 +4104,18 @@
         <v>412</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>413</v>
+        <v>402</v>
       </c>
     </row>
     <row r="201" spans="1:3" s="1" customFormat="1">
       <c r="A201" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B201" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="B201" s="4" t="s">
+      <c r="C201" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="C201" s="1" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="202" spans="1:3" s="1" customFormat="1">
@@ -4120,7 +4126,7 @@
         <v>417</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="203" spans="1:3" s="1" customFormat="1">
@@ -4131,7 +4137,7 @@
         <v>419</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="204" spans="1:3" s="1" customFormat="1">
@@ -4142,7 +4148,7 @@
         <v>421</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="205" spans="1:3" s="1" customFormat="1">
@@ -4153,7 +4159,7 @@
         <v>423</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="206" spans="1:3" s="1" customFormat="1">
@@ -4164,7 +4170,7 @@
         <v>425</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="207" spans="1:3" s="1" customFormat="1">
@@ -4175,7 +4181,7 @@
         <v>427</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="208" spans="1:3" s="1" customFormat="1">
@@ -4186,7 +4192,7 @@
         <v>429</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="209" spans="1:3" s="1" customFormat="1">
@@ -4197,7 +4203,7 @@
         <v>431</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="210" spans="1:3" s="1" customFormat="1">
@@ -4208,7 +4214,7 @@
         <v>433</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="211" spans="1:3" s="1" customFormat="1">
@@ -4219,7 +4225,7 @@
         <v>435</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="212" spans="1:3" s="1" customFormat="1">
@@ -4230,7 +4236,7 @@
         <v>437</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="213" spans="1:3" s="1" customFormat="1">
@@ -4241,7 +4247,7 @@
         <v>439</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="214" spans="1:3" s="1" customFormat="1">
@@ -4252,7 +4258,7 @@
         <v>441</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="215" spans="1:3" s="1" customFormat="1">
@@ -4263,7 +4269,7 @@
         <v>443</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="216" spans="1:3" s="1" customFormat="1">
@@ -4274,7 +4280,7 @@
         <v>445</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="217" spans="1:3" s="1" customFormat="1">
@@ -4285,7 +4291,7 @@
         <v>447</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="218" spans="1:3" s="1" customFormat="1">
@@ -4296,7 +4302,7 @@
         <v>449</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>168</v>
+        <v>353</v>
       </c>
     </row>
     <row r="219" spans="1:3" s="1" customFormat="1">
@@ -4307,7 +4313,7 @@
         <v>451</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="220" spans="1:3" s="1" customFormat="1">
@@ -4318,7 +4324,7 @@
         <v>453</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="221" spans="1:3" s="1" customFormat="1">
@@ -4329,7 +4335,7 @@
         <v>455</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="222" spans="1:3" s="1" customFormat="1">
@@ -4340,7 +4346,7 @@
         <v>457</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="223" spans="1:3" s="1" customFormat="1">
@@ -4351,7 +4357,7 @@
         <v>459</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="224" spans="1:3" s="1" customFormat="1">
@@ -4362,7 +4368,7 @@
         <v>461</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="225" spans="1:3" s="1" customFormat="1">
@@ -4373,7 +4379,7 @@
         <v>463</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="226" spans="1:3" s="1" customFormat="1">
@@ -4384,11 +4390,19 @@
         <v>465</v>
       </c>
       <c r="C226" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" s="1" customFormat="1">
+      <c r="A227" s="1" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="227" spans="1:3" s="1" customFormat="1">
-      <c r="B227"/>
+      <c r="B227" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="228" spans="1:3" s="1" customFormat="1">
       <c r="B228"/>
@@ -4492,8 +4506,11 @@
     <row r="261" spans="2:2" s="1" customFormat="1">
       <c r="B261"/>
     </row>
-    <row r="262" spans="2:2"/>
+    <row r="262" spans="2:2" s="1" customFormat="1">
+      <c r="B262"/>
+    </row>
     <row r="263" spans="2:2"/>
+    <row r="264" spans="2:2"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Feat]#79 fix filter error
</commit_message>
<xml_diff>
--- a/Projects/App/Resources/onboardingArtist.xlsx
+++ b/Projects/App/Resources/onboardingArtist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choihyowon/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E06DF69-3658-3E43-98D2-DEF01C49C229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA194540-ED5B-2F4A-B42E-FE8AFD7299EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{DDFC3EF1-0C9B-2449-839F-441E442BC4BA}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="통합(최종본)" sheetId="7" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'통합(최종본)'!$A$1:$C$262</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'통합(최종본)'!$B$1:$D$262</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1894,2623 +1894,3304 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF8B4FB7-ABFA-AA47-A964-F8732D4F461D}">
-  <dimension ref="A1:C264"/>
+  <dimension ref="A1:D264"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="164" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B225" sqref="B225"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="17.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+      <c r="D4" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
+      <c r="D5" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
+      <c r="D14" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
+      <c r="D18" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1" t="s">
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
+      <c r="D20" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
+        <v>21</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1" t="s">
+      <c r="D21" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1" t="s">
+      <c r="D22" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" s="1">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1" t="s">
+      <c r="D24" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1">
+        <v>25</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="1" t="s">
+      <c r="D25" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1">
+        <v>26</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:4">
+      <c r="A27" s="1">
+        <v>27</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1" t="s">
+      <c r="D27" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1">
+        <v>28</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:4">
+      <c r="A29" s="1">
+        <v>29</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:4">
+      <c r="A30" s="1">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:4">
+      <c r="A31" s="1">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:4">
+      <c r="A32" s="1">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:4">
+      <c r="A33" s="1">
+        <v>33</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:4">
+      <c r="A34" s="1">
+        <v>34</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="1" t="s">
+      <c r="D34" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1">
+        <v>35</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="1" t="s">
+      <c r="D35" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1">
+        <v>36</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="1" t="s">
+      <c r="D36" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
+        <v>37</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1" t="s">
+      <c r="D37" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
+        <v>38</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="1" t="s">
+      <c r="D38" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1">
+        <v>39</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="1" t="s">
+      <c r="D39" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1">
+        <v>40</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="1" t="s">
+      <c r="D40" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1">
+        <v>41</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="C41" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="1" t="s">
+      <c r="D41" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
+        <v>42</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="1" t="s">
+      <c r="D42" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
+        <v>43</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
+        <v>44</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="1" t="s">
+      <c r="D44" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
+        <v>45</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="1" t="s">
+      <c r="D45" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
+        <v>46</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="C46" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="1" t="s">
+      <c r="D46" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
+        <v>47</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="C47" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="1" t="s">
+      <c r="D47" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>48</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="1" t="s">
+      <c r="D48" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1">
+        <v>49</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="C49" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="1" t="s">
+      <c r="D49" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1">
+        <v>50</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="C50" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="1" t="s">
+      <c r="D50" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1">
+        <v>51</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="C51" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="1" t="s">
+      <c r="D51" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1">
+        <v>52</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="C52" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="1" t="s">
+      <c r="D52" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1">
+        <v>53</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="C53" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="1" t="s">
+      <c r="D53" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="1">
+        <v>54</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="C54" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="1" t="s">
+      <c r="D54" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1">
+        <v>55</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="C55" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="1" t="s">
+      <c r="D55" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1">
+        <v>56</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="C56" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="1" t="s">
+      <c r="D56" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="1">
+        <v>57</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="C57" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="1" t="s">
+      <c r="D57" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1">
+        <v>58</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="1" t="s">
+      <c r="D58" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="1">
+        <v>59</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="C59" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="1" t="s">
+      <c r="D59" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="1">
+        <v>60</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="C60" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="1" t="s">
+      <c r="D60" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="1">
+        <v>61</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="C61" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="1" t="s">
+      <c r="D61" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="1">
+        <v>62</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="C62" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="1" t="s">
+      <c r="D62" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="1">
+        <v>63</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="C63" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="1" t="s">
+      <c r="D63" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1">
+        <v>64</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="C64" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="1" t="s">
+      <c r="D64" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="1">
+        <v>65</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="C65" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="1" t="s">
+      <c r="D65" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="1">
+        <v>66</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="C66" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="1" t="s">
+      <c r="D66" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="1">
+        <v>67</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="C67" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="1" t="s">
+      <c r="D67" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="1">
+        <v>68</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="C68" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="1" t="s">
+      <c r="D68" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="1">
+        <v>69</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="C69" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="1" t="s">
+      <c r="D69" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="1">
+        <v>70</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="C70" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="1" t="s">
+      <c r="D70" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="1">
+        <v>71</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="C71" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="1" t="s">
+      <c r="D71" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="1">
+        <v>72</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="C72" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="1" t="s">
+      <c r="D72" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="1">
+        <v>73</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="C73" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="1" t="s">
+      <c r="D73" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="1">
+        <v>74</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:4">
+      <c r="A75" s="1">
+        <v>75</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="D75" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:4">
+      <c r="A76" s="1">
+        <v>76</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="1" t="s">
+    <row r="77" spans="1:4">
+      <c r="A77" s="1">
+        <v>77</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="D77" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="1" t="s">
+    <row r="78" spans="1:4">
+      <c r="A78" s="1">
+        <v>78</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:4">
+      <c r="A79" s="1">
+        <v>79</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="C79" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="D79" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="1" t="s">
+    <row r="80" spans="1:4">
+      <c r="A80" s="1">
+        <v>80</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="C80" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:4">
+      <c r="A81" s="1">
+        <v>81</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="C81" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="1" t="s">
+    <row r="82" spans="1:4">
+      <c r="A82" s="1">
+        <v>82</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="C82" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="1" t="s">
+    <row r="83" spans="1:4">
+      <c r="A83" s="1">
+        <v>83</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="C83" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="D83" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="84" spans="1:3" s="1" customFormat="1">
-      <c r="A84" s="1" t="s">
+    <row r="84" spans="1:4" s="1" customFormat="1">
+      <c r="A84" s="1">
+        <v>84</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="C84" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="85" spans="1:3" s="1" customFormat="1">
-      <c r="A85" s="1" t="s">
+    <row r="85" spans="1:4" s="1" customFormat="1">
+      <c r="A85" s="1">
+        <v>85</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="D85" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="86" spans="1:3" s="1" customFormat="1">
-      <c r="A86" s="1" t="s">
+    <row r="86" spans="1:4" s="1" customFormat="1">
+      <c r="A86" s="1">
+        <v>86</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="C86" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="D86" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="87" spans="1:3" s="1" customFormat="1">
-      <c r="A87" s="1" t="s">
+    <row r="87" spans="1:4" s="1" customFormat="1">
+      <c r="A87" s="1">
+        <v>87</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="C87" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="D87" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="88" spans="1:3" s="1" customFormat="1">
-      <c r="A88" s="1" t="s">
+    <row r="88" spans="1:4" s="1" customFormat="1">
+      <c r="A88" s="1">
+        <v>88</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="D88" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="89" spans="1:3" s="1" customFormat="1">
-      <c r="A89" s="1" t="s">
+    <row r="89" spans="1:4" s="1" customFormat="1">
+      <c r="A89" s="1">
+        <v>89</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="D89" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="90" spans="1:3" s="1" customFormat="1">
-      <c r="A90" s="1" t="s">
+    <row r="90" spans="1:4" s="1" customFormat="1">
+      <c r="A90" s="1">
+        <v>90</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="D90" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="91" spans="1:3" s="1" customFormat="1">
-      <c r="A91" s="1" t="s">
+    <row r="91" spans="1:4" s="1" customFormat="1">
+      <c r="A91" s="1">
+        <v>91</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="D91" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="92" spans="1:3" s="1" customFormat="1">
-      <c r="A92" s="1" t="s">
+    <row r="92" spans="1:4" s="1" customFormat="1">
+      <c r="A92" s="1">
+        <v>92</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="C92" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="D92" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="93" spans="1:3" s="1" customFormat="1">
-      <c r="A93" s="1" t="s">
+    <row r="93" spans="1:4" s="1" customFormat="1">
+      <c r="A93" s="1">
+        <v>93</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="D93" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="94" spans="1:3" s="1" customFormat="1">
-      <c r="A94" s="1" t="s">
+    <row r="94" spans="1:4" s="1" customFormat="1">
+      <c r="A94" s="1">
+        <v>94</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="C94" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="D94" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="95" spans="1:3" s="1" customFormat="1">
-      <c r="A95" s="1" t="s">
+    <row r="95" spans="1:4" s="1" customFormat="1">
+      <c r="A95" s="1">
+        <v>95</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="C95" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="D95" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="96" spans="1:3" s="1" customFormat="1">
-      <c r="A96" s="1" t="s">
+    <row r="96" spans="1:4" s="1" customFormat="1">
+      <c r="A96" s="1">
+        <v>96</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="D96" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="97" spans="1:3" s="1" customFormat="1">
-      <c r="A97" s="1" t="s">
+    <row r="97" spans="1:4" s="1" customFormat="1">
+      <c r="A97" s="1">
+        <v>97</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="C97" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="D97" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="98" spans="1:3" s="1" customFormat="1">
-      <c r="A98" s="1" t="s">
+    <row r="98" spans="1:4" s="1" customFormat="1">
+      <c r="A98" s="1">
+        <v>98</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="C98" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="D98" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="99" spans="1:3" s="1" customFormat="1">
-      <c r="A99" s="1" t="s">
+    <row r="99" spans="1:4" s="1" customFormat="1">
+      <c r="A99" s="1">
+        <v>99</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="C99" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="D99" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="100" spans="1:3" s="1" customFormat="1">
-      <c r="A100" s="1" t="s">
+    <row r="100" spans="1:4" s="1" customFormat="1">
+      <c r="A100" s="1">
+        <v>100</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="C100" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="D100" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="101" spans="1:3" s="1" customFormat="1">
-      <c r="A101" s="1" t="s">
+    <row r="101" spans="1:4" s="1" customFormat="1">
+      <c r="A101" s="1">
+        <v>101</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="D101" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="102" spans="1:3" s="1" customFormat="1">
-      <c r="A102" s="1" t="s">
+    <row r="102" spans="1:4" s="1" customFormat="1">
+      <c r="A102" s="1">
+        <v>102</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="D102" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="103" spans="1:3" s="1" customFormat="1">
-      <c r="A103" s="1" t="s">
+    <row r="103" spans="1:4" s="1" customFormat="1">
+      <c r="A103" s="1">
+        <v>103</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="D103" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="104" spans="1:3" s="1" customFormat="1">
-      <c r="A104" s="1" t="s">
+    <row r="104" spans="1:4" s="1" customFormat="1">
+      <c r="A104" s="1">
+        <v>104</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="C104" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="D104" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="105" spans="1:3" s="1" customFormat="1">
-      <c r="A105" s="1" t="s">
+    <row r="105" spans="1:4" s="1" customFormat="1">
+      <c r="A105" s="1">
+        <v>105</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="C105" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="D105" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="106" spans="1:3" s="1" customFormat="1">
-      <c r="A106" s="1" t="s">
+    <row r="106" spans="1:4" s="1" customFormat="1">
+      <c r="A106" s="1">
+        <v>106</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="C106" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="D106" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="107" spans="1:3" s="1" customFormat="1">
-      <c r="A107" s="1" t="s">
+    <row r="107" spans="1:4" s="1" customFormat="1">
+      <c r="A107" s="1">
+        <v>107</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="C107" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="D107" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="108" spans="1:3" s="1" customFormat="1">
-      <c r="A108" s="1" t="s">
+    <row r="108" spans="1:4" s="1" customFormat="1">
+      <c r="A108" s="1">
+        <v>108</v>
+      </c>
+      <c r="B108" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="C108" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="D108" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="109" spans="1:3" s="1" customFormat="1">
-      <c r="A109" s="1" t="s">
+    <row r="109" spans="1:4" s="1" customFormat="1">
+      <c r="A109" s="1">
+        <v>109</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="C109" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="D109" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="110" spans="1:3" s="1" customFormat="1">
-      <c r="A110" s="1" t="s">
+    <row r="110" spans="1:4" s="1" customFormat="1">
+      <c r="A110" s="1">
+        <v>110</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="C110" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="D110" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="111" spans="1:3" s="1" customFormat="1">
-      <c r="A111" s="1" t="s">
+    <row r="111" spans="1:4" s="1" customFormat="1">
+      <c r="A111" s="1">
+        <v>111</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="C111" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="D111" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="112" spans="1:3" s="1" customFormat="1">
-      <c r="A112" s="1" t="s">
+    <row r="112" spans="1:4" s="1" customFormat="1">
+      <c r="A112" s="1">
+        <v>112</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="C112" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="D112" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="113" spans="1:3" s="1" customFormat="1">
-      <c r="A113" s="1" t="s">
+    <row r="113" spans="1:4" s="1" customFormat="1">
+      <c r="A113" s="1">
+        <v>113</v>
+      </c>
+      <c r="B113" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="C113" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="D113" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="114" spans="1:3" s="1" customFormat="1">
-      <c r="A114" s="1" t="s">
+    <row r="114" spans="1:4" s="1" customFormat="1">
+      <c r="A114" s="1">
+        <v>114</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="C114" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="D114" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="115" spans="1:3" s="1" customFormat="1">
-      <c r="A115" s="1" t="s">
+    <row r="115" spans="1:4" s="1" customFormat="1">
+      <c r="A115" s="1">
+        <v>115</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="C115" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="D115" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="116" spans="1:3" s="1" customFormat="1">
-      <c r="A116" s="1" t="s">
+    <row r="116" spans="1:4" s="1" customFormat="1">
+      <c r="A116" s="1">
+        <v>116</v>
+      </c>
+      <c r="B116" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="C116" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="D116" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="117" spans="1:3" s="1" customFormat="1">
-      <c r="A117" s="1" t="s">
+    <row r="117" spans="1:4" s="1" customFormat="1">
+      <c r="A117" s="1">
+        <v>117</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="C117" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="D117" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="118" spans="1:3" s="1" customFormat="1">
-      <c r="A118" s="1" t="s">
+    <row r="118" spans="1:4" s="1" customFormat="1">
+      <c r="A118" s="1">
+        <v>118</v>
+      </c>
+      <c r="B118" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="C118" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="D118" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="119" spans="1:3" s="1" customFormat="1">
-      <c r="A119" s="1" t="s">
+    <row r="119" spans="1:4" s="1" customFormat="1">
+      <c r="A119" s="1">
+        <v>119</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="C119" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="D119" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="120" spans="1:3" s="1" customFormat="1">
-      <c r="A120" s="1" t="s">
+    <row r="120" spans="1:4" s="1" customFormat="1">
+      <c r="A120" s="1">
+        <v>120</v>
+      </c>
+      <c r="B120" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="C120" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="D120" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="121" spans="1:3" s="1" customFormat="1">
-      <c r="A121" s="1" t="s">
+    <row r="121" spans="1:4" s="1" customFormat="1">
+      <c r="A121" s="1">
+        <v>121</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="C121" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="D121" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="122" spans="1:3" s="1" customFormat="1">
-      <c r="A122" s="1" t="s">
+    <row r="122" spans="1:4" s="1" customFormat="1">
+      <c r="A122" s="1">
+        <v>122</v>
+      </c>
+      <c r="B122" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="C122" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="D122" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="123" spans="1:3" s="1" customFormat="1">
-      <c r="A123" s="1" t="s">
+    <row r="123" spans="1:4" s="1" customFormat="1">
+      <c r="A123" s="1">
+        <v>123</v>
+      </c>
+      <c r="B123" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="C123" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="C123" s="3" t="s">
+      <c r="D123" s="3" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="124" spans="1:3" s="1" customFormat="1">
-      <c r="A124" s="1" t="s">
+    <row r="124" spans="1:4" s="1" customFormat="1">
+      <c r="A124" s="1">
+        <v>124</v>
+      </c>
+      <c r="B124" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="C124" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C124" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" s="1" customFormat="1">
-      <c r="A125" s="1" t="s">
+      <c r="D124" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" s="1" customFormat="1">
+      <c r="A125" s="1">
+        <v>125</v>
+      </c>
+      <c r="B125" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="C125" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="D125" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="126" spans="1:3" s="1" customFormat="1">
-      <c r="A126" s="1" t="s">
+    <row r="126" spans="1:4" s="1" customFormat="1">
+      <c r="A126" s="1">
+        <v>126</v>
+      </c>
+      <c r="B126" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="C126" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="D126" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="127" spans="1:3" s="1" customFormat="1">
-      <c r="A127" s="1" t="s">
+    <row r="127" spans="1:4" s="1" customFormat="1">
+      <c r="A127" s="1">
+        <v>127</v>
+      </c>
+      <c r="B127" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="C127" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="D127" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="128" spans="1:3" s="1" customFormat="1">
-      <c r="A128" s="1" t="s">
+    <row r="128" spans="1:4" s="1" customFormat="1">
+      <c r="A128" s="1">
+        <v>128</v>
+      </c>
+      <c r="B128" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="C128" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="D128" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="129" spans="1:3" s="1" customFormat="1">
-      <c r="A129" s="1" t="s">
+    <row r="129" spans="1:4" s="1" customFormat="1">
+      <c r="A129" s="1">
+        <v>129</v>
+      </c>
+      <c r="B129" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="C129" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="D129" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="130" spans="1:3" s="1" customFormat="1">
-      <c r="A130" s="1" t="s">
+    <row r="130" spans="1:4" s="1" customFormat="1">
+      <c r="A130" s="1">
+        <v>130</v>
+      </c>
+      <c r="B130" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="C130" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="D130" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="131" spans="1:3" s="1" customFormat="1">
-      <c r="A131" s="1" t="s">
+    <row r="131" spans="1:4" s="1" customFormat="1">
+      <c r="A131" s="1">
+        <v>131</v>
+      </c>
+      <c r="B131" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="C131" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="D131" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="132" spans="1:3" s="1" customFormat="1">
-      <c r="A132" s="1" t="s">
+    <row r="132" spans="1:4" s="1" customFormat="1">
+      <c r="A132" s="1">
+        <v>132</v>
+      </c>
+      <c r="B132" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="C132" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C132" s="1" t="s">
+      <c r="D132" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="133" spans="1:3" s="1" customFormat="1">
-      <c r="A133" s="1" t="s">
+    <row r="133" spans="1:4" s="1" customFormat="1">
+      <c r="A133" s="1">
+        <v>133</v>
+      </c>
+      <c r="B133" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="C133" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="C133" s="1" t="s">
+      <c r="D133" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="134" spans="1:3" s="1" customFormat="1">
-      <c r="A134" s="1" t="s">
+    <row r="134" spans="1:4" s="1" customFormat="1">
+      <c r="A134" s="1">
+        <v>134</v>
+      </c>
+      <c r="B134" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B134" s="2" t="s">
+      <c r="C134" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="D134" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="135" spans="1:3" s="1" customFormat="1">
-      <c r="A135" s="1" t="s">
+    <row r="135" spans="1:4" s="1" customFormat="1">
+      <c r="A135" s="1">
+        <v>135</v>
+      </c>
+      <c r="B135" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="C135" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C135" s="1" t="s">
+      <c r="D135" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="136" spans="1:3" s="1" customFormat="1">
-      <c r="A136" s="1" t="s">
+    <row r="136" spans="1:4" s="1" customFormat="1">
+      <c r="A136" s="1">
+        <v>136</v>
+      </c>
+      <c r="B136" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="C136" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C136" s="1" t="s">
+      <c r="D136" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="137" spans="1:3" s="1" customFormat="1">
-      <c r="A137" s="1" t="s">
+    <row r="137" spans="1:4" s="1" customFormat="1">
+      <c r="A137" s="1">
+        <v>137</v>
+      </c>
+      <c r="B137" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="C137" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C137" s="1" t="s">
+      <c r="D137" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:3" s="1" customFormat="1">
-      <c r="A138" s="1" t="s">
+    <row r="138" spans="1:4" s="1" customFormat="1">
+      <c r="A138" s="1">
+        <v>138</v>
+      </c>
+      <c r="B138" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="C138" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="C138" s="1" t="s">
+      <c r="D138" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="139" spans="1:3" s="1" customFormat="1">
-      <c r="A139" s="1" t="s">
+    <row r="139" spans="1:4" s="1" customFormat="1">
+      <c r="A139" s="1">
+        <v>139</v>
+      </c>
+      <c r="B139" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="C139" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="D139" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="140" spans="1:3" s="1" customFormat="1">
-      <c r="A140" s="1" t="s">
+    <row r="140" spans="1:4" s="1" customFormat="1">
+      <c r="A140" s="1">
+        <v>140</v>
+      </c>
+      <c r="B140" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="C140" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="C140" s="1" t="s">
+      <c r="D140" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="141" spans="1:3" s="1" customFormat="1">
-      <c r="A141" s="1" t="s">
+    <row r="141" spans="1:4" s="1" customFormat="1">
+      <c r="A141" s="1">
+        <v>141</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="C141" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="C141" s="1" t="s">
+      <c r="D141" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="142" spans="1:3" s="1" customFormat="1">
-      <c r="A142" s="1" t="s">
+    <row r="142" spans="1:4" s="1" customFormat="1">
+      <c r="A142" s="1">
+        <v>142</v>
+      </c>
+      <c r="B142" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="C142" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="D142" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="143" spans="1:3" s="1" customFormat="1">
-      <c r="A143" s="1" t="s">
+    <row r="143" spans="1:4" s="1" customFormat="1">
+      <c r="A143" s="1">
+        <v>143</v>
+      </c>
+      <c r="B143" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="C143" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="C143" s="1" t="s">
+      <c r="D143" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="144" spans="1:3" s="1" customFormat="1">
-      <c r="A144" s="1" t="s">
+    <row r="144" spans="1:4" s="1" customFormat="1">
+      <c r="A144" s="1">
+        <v>144</v>
+      </c>
+      <c r="B144" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="C144" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C144" s="1" t="s">
+      <c r="D144" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="145" spans="1:3" s="1" customFormat="1">
-      <c r="A145" s="1" t="s">
+    <row r="145" spans="1:4" s="1" customFormat="1">
+      <c r="A145" s="1">
+        <v>145</v>
+      </c>
+      <c r="B145" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="C145" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C145" s="1" t="s">
+      <c r="D145" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="146" spans="1:3" s="1" customFormat="1">
-      <c r="A146" s="1" t="s">
+    <row r="146" spans="1:4" s="1" customFormat="1">
+      <c r="A146" s="1">
+        <v>146</v>
+      </c>
+      <c r="B146" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="C146" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="D146" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="147" spans="1:3" s="1" customFormat="1">
-      <c r="A147" s="1" t="s">
+    <row r="147" spans="1:4" s="1" customFormat="1">
+      <c r="A147" s="1">
+        <v>147</v>
+      </c>
+      <c r="B147" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="B147" s="2" t="s">
+      <c r="C147" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="C147" s="1" t="s">
+      <c r="D147" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="148" spans="1:3" s="1" customFormat="1">
-      <c r="A148" s="1" t="s">
+    <row r="148" spans="1:4" s="1" customFormat="1">
+      <c r="A148" s="1">
+        <v>148</v>
+      </c>
+      <c r="B148" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="B148" s="2" t="s">
+      <c r="C148" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="C148" s="1" t="s">
+      <c r="D148" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="149" spans="1:3" s="1" customFormat="1">
-      <c r="A149" s="1" t="s">
+    <row r="149" spans="1:4" s="1" customFormat="1">
+      <c r="A149" s="1">
+        <v>149</v>
+      </c>
+      <c r="B149" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B149" s="2" t="s">
+      <c r="C149" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="C149" s="1" t="s">
+      <c r="D149" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="150" spans="1:3" s="1" customFormat="1">
-      <c r="A150" s="1" t="s">
+    <row r="150" spans="1:4" s="1" customFormat="1">
+      <c r="A150" s="1">
+        <v>150</v>
+      </c>
+      <c r="B150" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="C150" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="C150" s="1" t="s">
+      <c r="D150" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="151" spans="1:3" s="1" customFormat="1">
-      <c r="A151" s="1" t="s">
+    <row r="151" spans="1:4" s="1" customFormat="1">
+      <c r="A151" s="1">
+        <v>151</v>
+      </c>
+      <c r="B151" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="C151" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="C151" s="1" t="s">
+      <c r="D151" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="152" spans="1:3" s="1" customFormat="1">
-      <c r="A152" s="1" t="s">
+    <row r="152" spans="1:4" s="1" customFormat="1">
+      <c r="A152" s="1">
+        <v>152</v>
+      </c>
+      <c r="B152" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="C152" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="C152" s="1" t="s">
+      <c r="D152" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="153" spans="1:3" s="1" customFormat="1">
-      <c r="A153" s="1" t="s">
+    <row r="153" spans="1:4" s="1" customFormat="1">
+      <c r="A153" s="1">
+        <v>153</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="C153" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C153" s="1" t="s">
+      <c r="D153" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="154" spans="1:3" s="1" customFormat="1">
-      <c r="A154" s="1" t="s">
+    <row r="154" spans="1:4" s="1" customFormat="1">
+      <c r="A154" s="1">
+        <v>154</v>
+      </c>
+      <c r="B154" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B154" s="2" t="s">
+      <c r="C154" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C154" s="1" t="s">
+      <c r="D154" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="155" spans="1:3" s="1" customFormat="1">
-      <c r="A155" s="1" t="s">
+    <row r="155" spans="1:4" s="1" customFormat="1">
+      <c r="A155" s="1">
+        <v>155</v>
+      </c>
+      <c r="B155" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="C155" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C155" s="1" t="s">
+      <c r="D155" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="156" spans="1:3" s="1" customFormat="1">
-      <c r="A156" s="1" t="s">
+    <row r="156" spans="1:4" s="1" customFormat="1">
+      <c r="A156" s="1">
+        <v>156</v>
+      </c>
+      <c r="B156" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="C156" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="C156" s="1" t="s">
+      <c r="D156" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="157" spans="1:3" s="1" customFormat="1">
-      <c r="A157" s="1" t="s">
+    <row r="157" spans="1:4" s="1" customFormat="1">
+      <c r="A157" s="1">
+        <v>157</v>
+      </c>
+      <c r="B157" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="C157" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="C157" s="1" t="s">
+      <c r="D157" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="158" spans="1:3" s="1" customFormat="1">
-      <c r="A158" s="1" t="s">
+    <row r="158" spans="1:4" s="1" customFormat="1">
+      <c r="A158" s="1">
+        <v>158</v>
+      </c>
+      <c r="B158" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B158" s="2" t="s">
+      <c r="C158" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="C158" s="1" t="s">
+      <c r="D158" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="159" spans="1:3" s="1" customFormat="1">
-      <c r="A159" s="1" t="s">
+    <row r="159" spans="1:4" s="1" customFormat="1">
+      <c r="A159" s="1">
+        <v>159</v>
+      </c>
+      <c r="B159" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="B159" s="2" t="s">
+      <c r="C159" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="C159" s="1" t="s">
+      <c r="D159" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="160" spans="1:3" s="1" customFormat="1">
-      <c r="A160" s="1" t="s">
+    <row r="160" spans="1:4" s="1" customFormat="1">
+      <c r="A160" s="1">
+        <v>160</v>
+      </c>
+      <c r="B160" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="B160" s="2" t="s">
+      <c r="C160" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="C160" s="1" t="s">
+      <c r="D160" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="161" spans="1:3" s="1" customFormat="1">
-      <c r="A161" s="1" t="s">
+    <row r="161" spans="1:4" s="1" customFormat="1">
+      <c r="A161" s="1">
+        <v>161</v>
+      </c>
+      <c r="B161" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B161" s="2" t="s">
+      <c r="C161" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C161" s="1" t="s">
+      <c r="D161" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="162" spans="1:3" s="1" customFormat="1">
-      <c r="A162" s="3" t="s">
+    <row r="162" spans="1:4" s="1" customFormat="1">
+      <c r="A162" s="1">
+        <v>162</v>
+      </c>
+      <c r="B162" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="B162" s="2" t="s">
+      <c r="C162" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="C162" s="1" t="s">
+      <c r="D162" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="163" spans="1:3" s="1" customFormat="1">
-      <c r="A163" s="1" t="s">
+    <row r="163" spans="1:4" s="1" customFormat="1">
+      <c r="A163" s="1">
+        <v>163</v>
+      </c>
+      <c r="B163" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B163" s="2" t="s">
+      <c r="C163" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="C163" s="1" t="s">
+      <c r="D163" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="164" spans="1:3" s="1" customFormat="1">
-      <c r="A164" s="1" t="s">
+    <row r="164" spans="1:4" s="1" customFormat="1">
+      <c r="A164" s="1">
+        <v>164</v>
+      </c>
+      <c r="B164" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="B164" s="2" t="s">
+      <c r="C164" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="C164" s="1" t="s">
+      <c r="D164" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="165" spans="1:3" s="1" customFormat="1">
-      <c r="A165" s="1" t="s">
+    <row r="165" spans="1:4" s="1" customFormat="1">
+      <c r="A165" s="1">
+        <v>165</v>
+      </c>
+      <c r="B165" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="B165" s="2" t="s">
+      <c r="C165" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="C165" s="1" t="s">
+      <c r="D165" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="166" spans="1:3" s="1" customFormat="1">
-      <c r="A166" s="1" t="s">
+    <row r="166" spans="1:4" s="1" customFormat="1">
+      <c r="A166" s="1">
+        <v>166</v>
+      </c>
+      <c r="B166" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="B166" s="2" t="s">
+      <c r="C166" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="C166" s="1" t="s">
+      <c r="D166" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="167" spans="1:3" s="1" customFormat="1">
-      <c r="A167" s="1" t="s">
+    <row r="167" spans="1:4" s="1" customFormat="1">
+      <c r="A167" s="1">
+        <v>167</v>
+      </c>
+      <c r="B167" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="B167" s="2" t="s">
+      <c r="C167" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="C167" s="1" t="s">
+      <c r="D167" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="168" spans="1:3" s="1" customFormat="1">
-      <c r="A168" s="1" t="s">
+    <row r="168" spans="1:4" s="1" customFormat="1">
+      <c r="A168" s="1">
+        <v>168</v>
+      </c>
+      <c r="B168" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B168" s="2" t="s">
+      <c r="C168" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="C168" s="1" t="s">
+      <c r="D168" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="169" spans="1:3" s="1" customFormat="1">
-      <c r="A169" s="1" t="s">
+    <row r="169" spans="1:4" s="1" customFormat="1">
+      <c r="A169" s="1">
+        <v>169</v>
+      </c>
+      <c r="B169" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="B169" s="2" t="s">
+      <c r="C169" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="C169" s="1" t="s">
+      <c r="D169" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="170" spans="1:3" s="1" customFormat="1">
-      <c r="A170" s="1" t="s">
+    <row r="170" spans="1:4" s="1" customFormat="1">
+      <c r="A170" s="1">
+        <v>170</v>
+      </c>
+      <c r="B170" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="B170" s="2" t="s">
+      <c r="C170" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="C170" s="1" t="s">
+      <c r="D170" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="171" spans="1:3" s="1" customFormat="1">
-      <c r="A171" s="1" t="s">
+    <row r="171" spans="1:4" s="1" customFormat="1">
+      <c r="A171" s="1">
+        <v>171</v>
+      </c>
+      <c r="B171" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="B171" s="2" t="s">
+      <c r="C171" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="C171" s="1" t="s">
+      <c r="D171" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="172" spans="1:3" s="1" customFormat="1">
-      <c r="A172" s="1" t="s">
+    <row r="172" spans="1:4" s="1" customFormat="1">
+      <c r="A172" s="1">
+        <v>172</v>
+      </c>
+      <c r="B172" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="B172" s="2" t="s">
+      <c r="C172" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="C172" s="1" t="s">
+      <c r="D172" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="173" spans="1:3" s="1" customFormat="1">
-      <c r="A173" s="1" t="s">
+    <row r="173" spans="1:4" s="1" customFormat="1">
+      <c r="A173" s="1">
+        <v>173</v>
+      </c>
+      <c r="B173" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="C173" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="C173" s="1" t="s">
+      <c r="D173" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="174" spans="1:3" s="1" customFormat="1">
-      <c r="A174" s="1" t="s">
+    <row r="174" spans="1:4" s="1" customFormat="1">
+      <c r="A174" s="1">
+        <v>174</v>
+      </c>
+      <c r="B174" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="B174" s="2" t="s">
+      <c r="C174" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="C174" s="1" t="s">
+      <c r="D174" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="175" spans="1:3" s="1" customFormat="1">
-      <c r="A175" s="1" t="s">
+    <row r="175" spans="1:4" s="1" customFormat="1">
+      <c r="A175" s="1">
+        <v>175</v>
+      </c>
+      <c r="B175" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="B175" s="2" t="s">
+      <c r="C175" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="C175" s="1" t="s">
+      <c r="D175" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="176" spans="1:3" s="1" customFormat="1">
-      <c r="A176" s="1" t="s">
+    <row r="176" spans="1:4" s="1" customFormat="1">
+      <c r="A176" s="1">
+        <v>176</v>
+      </c>
+      <c r="B176" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="B176" s="2" t="s">
+      <c r="C176" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="C176" s="1" t="s">
+      <c r="D176" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="177" spans="1:3" s="1" customFormat="1">
-      <c r="A177" s="1" t="s">
+    <row r="177" spans="1:4" s="1" customFormat="1">
+      <c r="A177" s="1">
+        <v>177</v>
+      </c>
+      <c r="B177" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="B177" s="2" t="s">
+      <c r="C177" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="C177" s="1" t="s">
+      <c r="D177" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="178" spans="1:3" s="1" customFormat="1">
-      <c r="A178" s="1" t="s">
+    <row r="178" spans="1:4" s="1" customFormat="1">
+      <c r="A178" s="1">
+        <v>178</v>
+      </c>
+      <c r="B178" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="B178" s="2" t="s">
+      <c r="C178" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="C178" s="1" t="s">
+      <c r="D178" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="179" spans="1:3" s="1" customFormat="1">
-      <c r="A179" s="1" t="s">
+    <row r="179" spans="1:4" s="1" customFormat="1">
+      <c r="A179" s="1">
+        <v>179</v>
+      </c>
+      <c r="B179" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="B179" s="2" t="s">
+      <c r="C179" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="C179" s="1" t="s">
+      <c r="D179" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="180" spans="1:3" s="1" customFormat="1">
-      <c r="A180" s="1" t="s">
+    <row r="180" spans="1:4" s="1" customFormat="1">
+      <c r="A180" s="1">
+        <v>180</v>
+      </c>
+      <c r="B180" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="B180" s="2" t="s">
+      <c r="C180" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="C180" s="1" t="s">
+      <c r="D180" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="181" spans="1:3" s="1" customFormat="1">
-      <c r="A181" s="1" t="s">
+    <row r="181" spans="1:4" s="1" customFormat="1">
+      <c r="A181" s="1">
+        <v>181</v>
+      </c>
+      <c r="B181" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="B181" s="2" t="s">
+      <c r="C181" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="C181" s="1" t="s">
+      <c r="D181" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="182" spans="1:3" s="1" customFormat="1">
-      <c r="A182" s="1" t="s">
+    <row r="182" spans="1:4" s="1" customFormat="1">
+      <c r="A182" s="1">
+        <v>182</v>
+      </c>
+      <c r="B182" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="B182" s="4" t="s">
+      <c r="C182" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="C182" s="1" t="s">
+      <c r="D182" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="183" spans="1:3" s="1" customFormat="1">
-      <c r="A183" s="1" t="s">
+    <row r="183" spans="1:4" s="1" customFormat="1">
+      <c r="A183" s="1">
+        <v>183</v>
+      </c>
+      <c r="B183" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="B183" s="4" t="s">
+      <c r="C183" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="C183" s="1" t="s">
+      <c r="D183" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="184" spans="1:3" s="1" customFormat="1">
-      <c r="A184" s="1" t="s">
+    <row r="184" spans="1:4" s="1" customFormat="1">
+      <c r="A184" s="1">
+        <v>184</v>
+      </c>
+      <c r="B184" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="B184" s="4" t="s">
+      <c r="C184" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="C184" s="1" t="s">
+      <c r="D184" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="185" spans="1:3" s="1" customFormat="1">
-      <c r="A185" s="1" t="s">
+    <row r="185" spans="1:4" s="1" customFormat="1">
+      <c r="A185" s="1">
+        <v>185</v>
+      </c>
+      <c r="B185" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="B185" s="4" t="s">
+      <c r="C185" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="C185" s="1" t="s">
+      <c r="D185" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="186" spans="1:3" s="1" customFormat="1">
-      <c r="A186" s="1" t="s">
+    <row r="186" spans="1:4" s="1" customFormat="1">
+      <c r="A186" s="1">
+        <v>186</v>
+      </c>
+      <c r="B186" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="B186" s="4" t="s">
+      <c r="C186" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="C186" s="1" t="s">
+      <c r="D186" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="187" spans="1:3" s="1" customFormat="1">
-      <c r="A187" s="1" t="s">
+    <row r="187" spans="1:4" s="1" customFormat="1">
+      <c r="A187" s="1">
+        <v>187</v>
+      </c>
+      <c r="B187" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="B187" s="4" t="s">
+      <c r="C187" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="C187" s="1" t="s">
+      <c r="D187" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="188" spans="1:3" s="1" customFormat="1">
-      <c r="A188" s="1" t="s">
+    <row r="188" spans="1:4" s="1" customFormat="1">
+      <c r="A188" s="1">
+        <v>188</v>
+      </c>
+      <c r="B188" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="B188" s="4" t="s">
+      <c r="C188" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="C188" s="1" t="s">
+      <c r="D188" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="189" spans="1:3" s="1" customFormat="1">
-      <c r="A189" s="1" t="s">
+    <row r="189" spans="1:4" s="1" customFormat="1">
+      <c r="A189" s="1">
+        <v>189</v>
+      </c>
+      <c r="B189" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="B189" s="4" t="s">
+      <c r="C189" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="C189" s="1" t="s">
+      <c r="D189" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="190" spans="1:3" s="1" customFormat="1">
-      <c r="A190" s="1" t="s">
+    <row r="190" spans="1:4" s="1" customFormat="1">
+      <c r="A190" s="1">
+        <v>190</v>
+      </c>
+      <c r="B190" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="B190" s="4" t="s">
+      <c r="C190" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="C190" s="1" t="s">
+      <c r="D190" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="191" spans="1:3" s="1" customFormat="1">
-      <c r="A191" s="1" t="s">
+    <row r="191" spans="1:4" s="1" customFormat="1">
+      <c r="A191" s="1">
+        <v>191</v>
+      </c>
+      <c r="B191" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="B191" s="4" t="s">
+      <c r="C191" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="C191" s="1" t="s">
+      <c r="D191" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="192" spans="1:3" s="1" customFormat="1">
-      <c r="A192" s="1" t="s">
+    <row r="192" spans="1:4" s="1" customFormat="1">
+      <c r="A192" s="1">
+        <v>192</v>
+      </c>
+      <c r="B192" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="B192" s="4" t="s">
+      <c r="C192" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="C192" s="1" t="s">
+      <c r="D192" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="193" spans="1:3" s="1" customFormat="1">
-      <c r="A193" s="1" t="s">
+    <row r="193" spans="1:4" s="1" customFormat="1">
+      <c r="A193" s="1">
+        <v>193</v>
+      </c>
+      <c r="B193" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="B193" s="4" t="s">
+      <c r="C193" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="C193" s="1" t="s">
+      <c r="D193" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="194" spans="1:3" s="1" customFormat="1">
-      <c r="A194" s="1" t="s">
+    <row r="194" spans="1:4" s="1" customFormat="1">
+      <c r="A194" s="1">
+        <v>194</v>
+      </c>
+      <c r="B194" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="B194" s="4" t="s">
+      <c r="C194" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="C194" s="1" t="s">
+      <c r="D194" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="195" spans="1:3" s="1" customFormat="1">
-      <c r="A195" s="1" t="s">
+    <row r="195" spans="1:4" s="1" customFormat="1">
+      <c r="A195" s="1">
+        <v>195</v>
+      </c>
+      <c r="B195" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="B195" s="4" t="s">
+      <c r="C195" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="C195" s="1" t="s">
+      <c r="D195" s="1" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="196" spans="1:3" s="1" customFormat="1">
-      <c r="A196" s="1" t="s">
+    <row r="196" spans="1:4" s="1" customFormat="1">
+      <c r="A196" s="1">
+        <v>196</v>
+      </c>
+      <c r="B196" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="B196" s="4" t="s">
+      <c r="C196" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="C196" s="1" t="s">
+      <c r="D196" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="197" spans="1:3" s="1" customFormat="1">
-      <c r="A197" s="1" t="s">
+    <row r="197" spans="1:4" s="1" customFormat="1">
+      <c r="A197" s="1">
+        <v>197</v>
+      </c>
+      <c r="B197" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="B197" s="4" t="s">
+      <c r="C197" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="C197" s="1" t="s">
+      <c r="D197" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="198" spans="1:3" s="1" customFormat="1">
-      <c r="A198" s="1" t="s">
+    <row r="198" spans="1:4" s="1" customFormat="1">
+      <c r="A198" s="1">
+        <v>198</v>
+      </c>
+      <c r="B198" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="B198" s="4" t="s">
+      <c r="C198" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="C198" s="1" t="s">
+      <c r="D198" s="1" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="199" spans="1:3" s="1" customFormat="1">
-      <c r="A199" s="1" t="s">
+    <row r="199" spans="1:4" s="1" customFormat="1">
+      <c r="A199" s="1">
+        <v>199</v>
+      </c>
+      <c r="B199" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="B199" s="4" t="s">
+      <c r="C199" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="C199" s="1" t="s">
+      <c r="D199" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="200" spans="1:3" s="1" customFormat="1">
-      <c r="A200" s="1" t="s">
+    <row r="200" spans="1:4" s="1" customFormat="1">
+      <c r="A200" s="1">
+        <v>200</v>
+      </c>
+      <c r="B200" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="B200" s="4" t="s">
+      <c r="C200" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="C200" s="1" t="s">
+      <c r="D200" s="1" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="201" spans="1:3" s="1" customFormat="1">
-      <c r="A201" s="1" t="s">
+    <row r="201" spans="1:4" s="1" customFormat="1">
+      <c r="A201" s="1">
+        <v>201</v>
+      </c>
+      <c r="B201" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="B201" s="4" t="s">
+      <c r="C201" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="C201" s="1" t="s">
+      <c r="D201" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="202" spans="1:3" s="1" customFormat="1">
-      <c r="A202" s="1" t="s">
+    <row r="202" spans="1:4" s="1" customFormat="1">
+      <c r="A202" s="1">
+        <v>202</v>
+      </c>
+      <c r="B202" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="B202" s="4" t="s">
+      <c r="C202" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="C202" s="1" t="s">
+      <c r="D202" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="203" spans="1:3" s="1" customFormat="1">
-      <c r="A203" s="1" t="s">
+    <row r="203" spans="1:4" s="1" customFormat="1">
+      <c r="A203" s="1">
+        <v>203</v>
+      </c>
+      <c r="B203" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="B203" s="4" t="s">
+      <c r="C203" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="C203" s="1" t="s">
+      <c r="D203" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="204" spans="1:3" s="1" customFormat="1">
-      <c r="A204" s="1" t="s">
+    <row r="204" spans="1:4" s="1" customFormat="1">
+      <c r="A204" s="1">
+        <v>204</v>
+      </c>
+      <c r="B204" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="B204" s="4" t="s">
+      <c r="C204" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="C204" s="1" t="s">
+      <c r="D204" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="205" spans="1:3" s="1" customFormat="1">
-      <c r="A205" s="1" t="s">
+    <row r="205" spans="1:4" s="1" customFormat="1">
+      <c r="A205" s="1">
+        <v>205</v>
+      </c>
+      <c r="B205" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="B205" s="4" t="s">
+      <c r="C205" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="C205" s="1" t="s">
+      <c r="D205" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="206" spans="1:3" s="1" customFormat="1">
-      <c r="A206" s="1" t="s">
+    <row r="206" spans="1:4" s="1" customFormat="1">
+      <c r="A206" s="1">
+        <v>206</v>
+      </c>
+      <c r="B206" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="B206" s="4" t="s">
+      <c r="C206" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="C206" s="1" t="s">
+      <c r="D206" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="207" spans="1:3" s="1" customFormat="1">
-      <c r="A207" s="1" t="s">
+    <row r="207" spans="1:4" s="1" customFormat="1">
+      <c r="A207" s="1">
+        <v>207</v>
+      </c>
+      <c r="B207" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="B207" s="4" t="s">
+      <c r="C207" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="C207" s="1" t="s">
+      <c r="D207" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="208" spans="1:3" s="1" customFormat="1">
-      <c r="A208" s="1" t="s">
+    <row r="208" spans="1:4" s="1" customFormat="1">
+      <c r="A208" s="1">
+        <v>208</v>
+      </c>
+      <c r="B208" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="B208" s="4" t="s">
+      <c r="C208" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="C208" s="1" t="s">
+      <c r="D208" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="209" spans="1:3" s="1" customFormat="1">
-      <c r="A209" s="1" t="s">
+    <row r="209" spans="1:4" s="1" customFormat="1">
+      <c r="A209" s="1">
+        <v>209</v>
+      </c>
+      <c r="B209" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="B209" s="4" t="s">
+      <c r="C209" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="C209" s="1" t="s">
+      <c r="D209" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="210" spans="1:3" s="1" customFormat="1">
-      <c r="A210" s="1" t="s">
+    <row r="210" spans="1:4" s="1" customFormat="1">
+      <c r="A210" s="1">
+        <v>210</v>
+      </c>
+      <c r="B210" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="B210" s="4" t="s">
+      <c r="C210" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="C210" s="1" t="s">
+      <c r="D210" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="211" spans="1:3" s="1" customFormat="1">
-      <c r="A211" s="1" t="s">
+    <row r="211" spans="1:4" s="1" customFormat="1">
+      <c r="A211" s="1">
+        <v>211</v>
+      </c>
+      <c r="B211" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="B211" s="4" t="s">
+      <c r="C211" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="C211" s="1" t="s">
+      <c r="D211" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="212" spans="1:3" s="1" customFormat="1">
-      <c r="A212" s="1" t="s">
+    <row r="212" spans="1:4" s="1" customFormat="1">
+      <c r="A212" s="1">
+        <v>212</v>
+      </c>
+      <c r="B212" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="B212" s="4" t="s">
+      <c r="C212" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="C212" s="1" t="s">
+      <c r="D212" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="213" spans="1:3" s="1" customFormat="1">
-      <c r="A213" s="1" t="s">
+    <row r="213" spans="1:4" s="1" customFormat="1">
+      <c r="A213" s="1">
+        <v>213</v>
+      </c>
+      <c r="B213" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="B213" s="4" t="s">
+      <c r="C213" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="C213" s="1" t="s">
+      <c r="D213" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="214" spans="1:3" s="1" customFormat="1">
-      <c r="A214" s="1" t="s">
+    <row r="214" spans="1:4" s="1" customFormat="1">
+      <c r="A214" s="1">
+        <v>214</v>
+      </c>
+      <c r="B214" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="B214" s="4" t="s">
+      <c r="C214" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="C214" s="1" t="s">
+      <c r="D214" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="215" spans="1:3" s="1" customFormat="1">
-      <c r="A215" s="1" t="s">
+    <row r="215" spans="1:4" s="1" customFormat="1">
+      <c r="A215" s="1">
+        <v>215</v>
+      </c>
+      <c r="B215" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="B215" s="4" t="s">
+      <c r="C215" s="4" t="s">
         <v>443</v>
       </c>
-      <c r="C215" s="1" t="s">
+      <c r="D215" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="216" spans="1:3" s="1" customFormat="1">
-      <c r="A216" s="1" t="s">
+    <row r="216" spans="1:4" s="1" customFormat="1">
+      <c r="A216" s="1">
+        <v>216</v>
+      </c>
+      <c r="B216" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="B216" s="4" t="s">
+      <c r="C216" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="C216" s="1" t="s">
+      <c r="D216" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="217" spans="1:3" s="1" customFormat="1">
-      <c r="A217" s="1" t="s">
+    <row r="217" spans="1:4" s="1" customFormat="1">
+      <c r="A217" s="1">
+        <v>217</v>
+      </c>
+      <c r="B217" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="B217" s="4" t="s">
+      <c r="C217" s="4" t="s">
         <v>447</v>
       </c>
-      <c r="C217" s="1" t="s">
+      <c r="D217" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="218" spans="1:3" s="1" customFormat="1">
-      <c r="A218" s="1" t="s">
+    <row r="218" spans="1:4" s="1" customFormat="1">
+      <c r="A218" s="1">
+        <v>218</v>
+      </c>
+      <c r="B218" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="B218" s="4" t="s">
+      <c r="C218" s="4" t="s">
         <v>449</v>
       </c>
-      <c r="C218" s="1" t="s">
+      <c r="D218" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="219" spans="1:3" s="1" customFormat="1">
-      <c r="A219" s="1" t="s">
+    <row r="219" spans="1:4" s="1" customFormat="1">
+      <c r="A219" s="1">
+        <v>219</v>
+      </c>
+      <c r="B219" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="B219" s="4" t="s">
+      <c r="C219" s="4" t="s">
         <v>451</v>
       </c>
-      <c r="C219" s="1" t="s">
+      <c r="D219" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="220" spans="1:3" s="1" customFormat="1">
-      <c r="A220" s="1" t="s">
+    <row r="220" spans="1:4" s="1" customFormat="1">
+      <c r="A220" s="1">
+        <v>220</v>
+      </c>
+      <c r="B220" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="B220" s="4" t="s">
+      <c r="C220" s="4" t="s">
         <v>453</v>
       </c>
-      <c r="C220" s="1" t="s">
+      <c r="D220" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="221" spans="1:3" s="1" customFormat="1">
-      <c r="A221" s="1" t="s">
+    <row r="221" spans="1:4" s="1" customFormat="1">
+      <c r="A221" s="1">
+        <v>221</v>
+      </c>
+      <c r="B221" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="B221" s="4" t="s">
+      <c r="C221" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="C221" s="1" t="s">
+      <c r="D221" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="222" spans="1:3" s="1" customFormat="1">
-      <c r="A222" s="1" t="s">
+    <row r="222" spans="1:4" s="1" customFormat="1">
+      <c r="A222" s="1">
+        <v>222</v>
+      </c>
+      <c r="B222" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="B222" s="4" t="s">
+      <c r="C222" s="4" t="s">
         <v>457</v>
       </c>
-      <c r="C222" s="1" t="s">
+      <c r="D222" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="223" spans="1:3" s="1" customFormat="1">
-      <c r="A223" s="1" t="s">
+    <row r="223" spans="1:4" s="1" customFormat="1">
+      <c r="A223" s="1">
+        <v>223</v>
+      </c>
+      <c r="B223" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="B223" s="4" t="s">
+      <c r="C223" s="4" t="s">
         <v>459</v>
       </c>
-      <c r="C223" s="1" t="s">
+      <c r="D223" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="224" spans="1:3" s="1" customFormat="1">
-      <c r="A224" s="1" t="s">
+    <row r="224" spans="1:4" s="1" customFormat="1">
+      <c r="A224" s="1">
+        <v>224</v>
+      </c>
+      <c r="B224" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="B224" s="4" t="s">
+      <c r="C224" s="4" t="s">
         <v>461</v>
       </c>
-      <c r="C224" s="1" t="s">
+      <c r="D224" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="225" spans="1:3" s="1" customFormat="1">
-      <c r="A225" s="1" t="s">
+    <row r="225" spans="1:4" s="1" customFormat="1">
+      <c r="A225" s="1">
+        <v>225</v>
+      </c>
+      <c r="B225" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="B225" s="4" t="s">
+      <c r="C225" s="4" t="s">
         <v>463</v>
       </c>
-      <c r="C225" s="1" t="s">
+      <c r="D225" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="226" spans="1:3" s="1" customFormat="1">
-      <c r="A226" s="1" t="s">
+    <row r="226" spans="1:4" s="1" customFormat="1">
+      <c r="A226" s="1">
+        <v>226</v>
+      </c>
+      <c r="B226" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="B226" s="4" t="s">
+      <c r="C226" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="C226" s="1" t="s">
+      <c r="D226" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="227" spans="1:3" s="1" customFormat="1">
-      <c r="A227" s="1" t="s">
+    <row r="227" spans="1:4" s="1" customFormat="1">
+      <c r="A227" s="1">
+        <v>227</v>
+      </c>
+      <c r="B227" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="B227" s="4" t="s">
+      <c r="C227" s="4" t="s">
         <v>467</v>
       </c>
-      <c r="C227" s="1" t="s">
+      <c r="D227" s="1" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="228" spans="1:3" s="1" customFormat="1">
-      <c r="B228"/>
-    </row>
-    <row r="229" spans="1:3" s="1" customFormat="1">
-      <c r="B229"/>
-    </row>
-    <row r="230" spans="1:3" s="1" customFormat="1">
-      <c r="B230"/>
-    </row>
-    <row r="231" spans="1:3" s="1" customFormat="1">
-      <c r="B231"/>
-    </row>
-    <row r="232" spans="1:3" s="1" customFormat="1">
-      <c r="B232"/>
-    </row>
-    <row r="233" spans="1:3" s="1" customFormat="1">
-      <c r="B233"/>
-    </row>
-    <row r="234" spans="1:3" s="1" customFormat="1">
-      <c r="B234"/>
-    </row>
-    <row r="235" spans="1:3" s="1" customFormat="1">
-      <c r="B235"/>
-    </row>
-    <row r="236" spans="1:3" s="1" customFormat="1">
-      <c r="B236"/>
-    </row>
-    <row r="237" spans="1:3" s="1" customFormat="1">
-      <c r="B237"/>
-    </row>
-    <row r="238" spans="1:3" s="1" customFormat="1">
-      <c r="B238"/>
-    </row>
-    <row r="239" spans="1:3" s="1" customFormat="1">
-      <c r="B239"/>
-    </row>
-    <row r="240" spans="1:3" s="1" customFormat="1">
-      <c r="B240"/>
-    </row>
-    <row r="241" spans="2:2" s="1" customFormat="1">
-      <c r="B241"/>
-    </row>
-    <row r="242" spans="2:2" s="1" customFormat="1">
-      <c r="B242"/>
-    </row>
-    <row r="243" spans="2:2" s="1" customFormat="1">
-      <c r="B243"/>
-    </row>
-    <row r="244" spans="2:2" s="1" customFormat="1">
-      <c r="B244"/>
-    </row>
-    <row r="245" spans="2:2" s="1" customFormat="1">
-      <c r="B245"/>
-    </row>
-    <row r="246" spans="2:2" s="1" customFormat="1">
-      <c r="B246"/>
-    </row>
-    <row r="247" spans="2:2" s="1" customFormat="1">
-      <c r="B247"/>
-    </row>
-    <row r="248" spans="2:2" s="1" customFormat="1">
-      <c r="B248"/>
-    </row>
-    <row r="249" spans="2:2" s="1" customFormat="1">
-      <c r="B249"/>
-    </row>
-    <row r="250" spans="2:2" s="1" customFormat="1">
-      <c r="B250"/>
-    </row>
-    <row r="251" spans="2:2" s="1" customFormat="1">
-      <c r="B251"/>
-    </row>
-    <row r="252" spans="2:2" s="1" customFormat="1">
-      <c r="B252"/>
-    </row>
-    <row r="253" spans="2:2" s="1" customFormat="1">
-      <c r="B253"/>
-    </row>
-    <row r="254" spans="2:2" s="1" customFormat="1">
-      <c r="B254"/>
-    </row>
-    <row r="255" spans="2:2" s="1" customFormat="1">
-      <c r="B255"/>
-    </row>
-    <row r="256" spans="2:2" s="1" customFormat="1">
-      <c r="B256"/>
-    </row>
-    <row r="257" spans="2:2" s="1" customFormat="1">
-      <c r="B257"/>
-    </row>
-    <row r="258" spans="2:2" s="1" customFormat="1">
-      <c r="B258"/>
-    </row>
-    <row r="259" spans="2:2" s="1" customFormat="1">
-      <c r="B259"/>
-    </row>
-    <row r="260" spans="2:2" s="1" customFormat="1">
-      <c r="B260"/>
-    </row>
-    <row r="261" spans="2:2" s="1" customFormat="1">
-      <c r="B261"/>
-    </row>
-    <row r="262" spans="2:2" s="1" customFormat="1">
-      <c r="B262"/>
-    </row>
-    <row r="263" spans="2:2"/>
-    <row r="264" spans="2:2"/>
+    <row r="228" spans="1:4" s="1" customFormat="1">
+      <c r="C228"/>
+    </row>
+    <row r="229" spans="1:4" s="1" customFormat="1">
+      <c r="C229"/>
+    </row>
+    <row r="230" spans="1:4" s="1" customFormat="1">
+      <c r="C230"/>
+    </row>
+    <row r="231" spans="1:4" s="1" customFormat="1">
+      <c r="C231"/>
+    </row>
+    <row r="232" spans="1:4" s="1" customFormat="1">
+      <c r="C232"/>
+    </row>
+    <row r="233" spans="1:4" s="1" customFormat="1">
+      <c r="C233"/>
+    </row>
+    <row r="234" spans="1:4" s="1" customFormat="1">
+      <c r="C234"/>
+    </row>
+    <row r="235" spans="1:4" s="1" customFormat="1">
+      <c r="C235"/>
+    </row>
+    <row r="236" spans="1:4" s="1" customFormat="1">
+      <c r="C236"/>
+    </row>
+    <row r="237" spans="1:4" s="1" customFormat="1">
+      <c r="C237"/>
+    </row>
+    <row r="238" spans="1:4" s="1" customFormat="1">
+      <c r="C238"/>
+    </row>
+    <row r="239" spans="1:4" s="1" customFormat="1">
+      <c r="C239"/>
+    </row>
+    <row r="240" spans="1:4" s="1" customFormat="1">
+      <c r="C240"/>
+    </row>
+    <row r="241" spans="3:3" s="1" customFormat="1">
+      <c r="C241"/>
+    </row>
+    <row r="242" spans="3:3" s="1" customFormat="1">
+      <c r="C242"/>
+    </row>
+    <row r="243" spans="3:3" s="1" customFormat="1">
+      <c r="C243"/>
+    </row>
+    <row r="244" spans="3:3" s="1" customFormat="1">
+      <c r="C244"/>
+    </row>
+    <row r="245" spans="3:3" s="1" customFormat="1">
+      <c r="C245"/>
+    </row>
+    <row r="246" spans="3:3" s="1" customFormat="1">
+      <c r="C246"/>
+    </row>
+    <row r="247" spans="3:3" s="1" customFormat="1">
+      <c r="C247"/>
+    </row>
+    <row r="248" spans="3:3" s="1" customFormat="1">
+      <c r="C248"/>
+    </row>
+    <row r="249" spans="3:3" s="1" customFormat="1">
+      <c r="C249"/>
+    </row>
+    <row r="250" spans="3:3" s="1" customFormat="1">
+      <c r="C250"/>
+    </row>
+    <row r="251" spans="3:3" s="1" customFormat="1">
+      <c r="C251"/>
+    </row>
+    <row r="252" spans="3:3" s="1" customFormat="1">
+      <c r="C252"/>
+    </row>
+    <row r="253" spans="3:3" s="1" customFormat="1">
+      <c r="C253"/>
+    </row>
+    <row r="254" spans="3:3" s="1" customFormat="1">
+      <c r="C254"/>
+    </row>
+    <row r="255" spans="3:3" s="1" customFormat="1">
+      <c r="C255"/>
+    </row>
+    <row r="256" spans="3:3" s="1" customFormat="1">
+      <c r="C256"/>
+    </row>
+    <row r="257" spans="3:3" s="1" customFormat="1">
+      <c r="C257"/>
+    </row>
+    <row r="258" spans="3:3" s="1" customFormat="1">
+      <c r="C258"/>
+    </row>
+    <row r="259" spans="3:3" s="1" customFormat="1">
+      <c r="C259"/>
+    </row>
+    <row r="260" spans="3:3" s="1" customFormat="1">
+      <c r="C260"/>
+    </row>
+    <row r="261" spans="3:3" s="1" customFormat="1">
+      <c r="C261"/>
+    </row>
+    <row r="262" spans="3:3" s="1" customFormat="1">
+      <c r="C262"/>
+    </row>
+    <row r="263" spans="3:3"/>
+    <row r="264" spans="3:3"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Fix]#79 - complete data  onboarding to main
</commit_message>
<xml_diff>
--- a/Projects/App/Resources/onboardingArtist.xlsx
+++ b/Projects/App/Resources/onboardingArtist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choihyowon/Desktop/2023/ADA/Mac/Setlist/Projects/App/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE9A70A-46E9-4940-9B85-8FC4D2A65A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8E34FC-B028-534A-9FDD-FCB1868000C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15640" xr2:uid="{DDFC3EF1-0C9B-2449-839F-441E442BC4BA}"/>
   </bookViews>
@@ -385,9 +385,6 @@
     <t>745c5b92-325f-451d-bd52-e6b95229c776</t>
   </si>
   <si>
-    <t>Lany</t>
-  </si>
-  <si>
     <t>f1cc066a-6dd1-4b18-ae68-3708472ab4b1 </t>
   </si>
   <si>
@@ -616,10 +613,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>박재범 (Jay Park)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3dda8202-ce15-4031-862a-77bc6759d15e</t>
   </si>
   <si>
@@ -687,6 +680,14 @@
   </si>
   <si>
     <t>Central Cee</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jay Park</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LANY</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1125,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A18E46-C40A-D44C-92D2-00EB00D6AF41}">
   <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="17.25" customHeight="1"/>
@@ -1229,16 +1230,16 @@
     </row>
     <row r="7" spans="1:5" ht="20">
       <c r="A7" s="2" t="s">
-        <v>182</v>
+        <v>203</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C7" s="4">
         <v>11593</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -1319,76 +1320,76 @@
     </row>
     <row r="13" spans="1:5" ht="20">
       <c r="A13" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="C13" s="4">
         <v>326362</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" ht="20">
       <c r="A14" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="C14" s="4">
         <v>250301</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" ht="20">
       <c r="A15" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>149</v>
       </c>
       <c r="C15" s="4">
         <v>1177</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="20">
       <c r="A16" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>132</v>
       </c>
       <c r="C16" s="4">
         <v>43383</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" ht="20">
       <c r="A17" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>180</v>
       </c>
       <c r="C17" s="4">
         <v>24364</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E17" s="2"/>
     </row>
@@ -1439,46 +1440,46 @@
     </row>
     <row r="21" spans="1:5" ht="20">
       <c r="A21" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C21" s="4">
         <v>39141</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="20">
       <c r="A22" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C22" s="4">
         <v>297553</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" ht="20">
       <c r="A23" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C23" s="4">
         <v>217593</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E23" s="2"/>
     </row>
@@ -1544,61 +1545,61 @@
     </row>
     <row r="28" spans="1:5" ht="20">
       <c r="A28" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>140</v>
       </c>
       <c r="C28" s="4">
         <v>26507</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" ht="20">
       <c r="A29" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>142</v>
       </c>
       <c r="C29" s="4">
         <v>22457</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" ht="20">
       <c r="A30" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>144</v>
       </c>
       <c r="C30" s="4">
         <v>338777</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" ht="20">
       <c r="A31" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>177</v>
       </c>
       <c r="C31" s="4">
         <v>12024</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E31" s="2"/>
     </row>
@@ -1676,16 +1677,16 @@
     </row>
     <row r="37" spans="1:5" ht="20">
       <c r="A37" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>146</v>
       </c>
       <c r="C37" s="4">
         <v>1546645</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="20">
@@ -1961,114 +1962,114 @@
     </row>
     <row r="57" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A57" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="C57" s="4">
         <v>247886</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A58" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>113</v>
       </c>
       <c r="C58" s="4">
         <v>621686</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A59" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>115</v>
       </c>
       <c r="C59" s="4">
         <v>383998</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A60" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="C60" s="4">
         <v>8351</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A61" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="C61" s="4">
         <v>29472</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A62" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>122</v>
       </c>
       <c r="C62" s="4">
         <v>45824</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A63" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="C63" s="4">
         <v>13539</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A64" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="C64" s="4">
         <v>164661</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="65" spans="1:4" s="1" customFormat="1" ht="20">
@@ -2115,282 +2116,282 @@
     </row>
     <row r="68" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A68" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="C68" s="4">
         <v>615550</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="69" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A69" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>136</v>
       </c>
       <c r="C69" s="4">
         <v>12418</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="70" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A70" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="C70" s="4">
         <v>500</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="71" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A71" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B71" s="5" t="s">
         <v>152</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>153</v>
       </c>
       <c r="C71" s="4">
         <v>161507</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A72" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>155</v>
       </c>
       <c r="C72" s="4">
         <v>1090113</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="73" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A73" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B73" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>157</v>
       </c>
       <c r="C73" s="4">
         <v>2358</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="74" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A74" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C74" s="4">
         <v>897106</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="75" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A75" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>151</v>
       </c>
       <c r="C75" s="4">
         <v>2270044</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="76" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A76" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C76" s="4">
         <v>1825718</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="77" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A77" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C77" s="4">
         <v>672794</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="78" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A78" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C78" s="4">
         <v>988518</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="79" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A79" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B79" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>159</v>
       </c>
       <c r="C79" s="4">
         <v>139478</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A80" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B80" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>161</v>
       </c>
       <c r="C80" s="4">
         <v>296675</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="81" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A81" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B81" s="5" t="s">
         <v>162</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>163</v>
       </c>
       <c r="C81" s="4">
         <v>195029</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A82" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B82" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>165</v>
       </c>
       <c r="C82" s="4">
         <v>45</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A83" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B83" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>167</v>
       </c>
       <c r="C83" s="4">
         <v>1219340</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A84" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B84" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="C84" s="4">
         <v>130</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A85" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B85" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>171</v>
       </c>
       <c r="C85" s="4">
         <v>555561</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A86" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B86" s="5" t="s">
         <v>172</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>173</v>
       </c>
       <c r="C86" s="4">
         <v>1599675</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="87" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A87" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B87" s="5" t="s">
         <v>174</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>175</v>
       </c>
       <c r="C87" s="4">
         <v>2300</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="88" spans="1:5" s="1" customFormat="1" ht="20">
@@ -2433,15 +2434,15 @@
         <v>1008975</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="91" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A91" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C91" s="4">
         <v>11864</v>
@@ -2452,45 +2453,45 @@
     </row>
     <row r="92" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A92" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C92" s="4">
         <v>1639884</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="93" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A93" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C93" s="4">
         <v>2043567</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E93" s="2"/>
     </row>
     <row r="94" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A94" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C94" s="4">
         <v>1767632</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="1" customFormat="1" ht="20">

</xml_diff>

<commit_message>
[Feat]#79 - complete onboardingView
</commit_message>
<xml_diff>
--- a/Projects/App/Resources/onboardingArtist.xlsx
+++ b/Projects/App/Resources/onboardingArtist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choihyowon/Desktop/2023/ADA/Mac/Setlist/Projects/App/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8E34FC-B028-534A-9FDD-FCB1868000C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D32655-41CB-CE4B-83F7-8C269F695B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15640" xr2:uid="{DDFC3EF1-0C9B-2449-839F-441E442BC4BA}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="장르별 30명씩" sheetId="9" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'장르별 30명씩'!$A$18:$D$127</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'장르별 30명씩'!$A$18:$D$126</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="203">
   <si>
     <t>카더가든</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -52,9 +52,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Paul Kim</t>
-  </si>
-  <si>
     <t>8968d1ad-c830-4ab2-92d2-bd6bea0b6f42</t>
   </si>
   <si>
@@ -87,25 +84,16 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">dea836e0-66dd-4285-9cab-2272bcda93b8 </t>
-  </si>
-  <si>
     <t>밴드</t>
   </si>
   <si>
     <t>넬</t>
   </si>
   <si>
-    <t xml:space="preserve">e156615d-3ddd-4491-9584-4b9d971472c4 </t>
-  </si>
-  <si>
     <t>DAY6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">77191d5f-1045-4b3b-ad7f-12ea398db929 </t>
-  </si>
-  <si>
     <t>밴드</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -114,9 +102,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">730182f9-2b25-45cc-857a-054c2bbe8ade </t>
-  </si>
-  <si>
     <t>자우림</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -153,542 +138,545 @@
     <t>717d466b-36b8-4a43-86e9-e8b8c4a658d7</t>
   </si>
   <si>
-    <t>wave to earth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">89e95aa3-bd49-4af3-9c87-0d88b2093bb0 </t>
-  </si>
-  <si>
     <t>혁오</t>
   </si>
   <si>
-    <t xml:space="preserve">f619b92a-a1b5-481c-8405-df35fb7846f1 </t>
-  </si>
-  <si>
     <t>인디</t>
   </si>
   <si>
     <t>검정치마</t>
   </si>
   <si>
-    <t xml:space="preserve">a697464c-69b1-4bbc-88cc-570c025a25e5 </t>
-  </si>
-  <si>
     <t>아이유</t>
   </si>
   <si>
+    <t>인디</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>볼빨간사춘기</t>
+  </si>
+  <si>
+    <t>3529da27-3a5d-45bb-9308-4d131132a21e</t>
+  </si>
+  <si>
+    <t>백예린</t>
+  </si>
+  <si>
+    <t>d598652a-b64a-4e21-b607-bcec71698731</t>
+  </si>
+  <si>
+    <t>스텔라장</t>
+  </si>
+  <si>
+    <t>ece1a668-010c-4d2e-ad35-9985c950c320</t>
+  </si>
+  <si>
+    <t>헤이즈</t>
+  </si>
+  <si>
+    <t>8cea34d9-e1a5-4a92-87da-de947f741fe6</t>
+  </si>
+  <si>
+    <t>pH-1</t>
+  </si>
+  <si>
+    <t>투모로우바이투게더</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>케이팝</t>
+  </si>
+  <si>
+    <t>세븐틴</t>
+  </si>
+  <si>
+    <t>BTS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스타엑스</t>
+  </si>
+  <si>
+    <t>엔하이픈</t>
+  </si>
+  <si>
+    <t>더보이즈</t>
+  </si>
+  <si>
+    <t>SHINee</t>
+  </si>
+  <si>
+    <t>IVE</t>
+  </si>
+  <si>
+    <t>NewJeans</t>
+  </si>
+  <si>
+    <t>(여자)아이들</t>
+  </si>
+  <si>
+    <t>aespa</t>
+  </si>
+  <si>
+    <t>STAYC</t>
+  </si>
+  <si>
+    <t>BLACKPINK</t>
+  </si>
+  <si>
+    <t>ITZY</t>
+  </si>
+  <si>
+    <t>TWICE</t>
+  </si>
+  <si>
+    <t>NMIXX</t>
+  </si>
+  <si>
+    <t>마마무</t>
+  </si>
+  <si>
+    <t>WOODZ</t>
+  </si>
+  <si>
+    <t>25c73c37-9517-4144-8ef6-32541e82ff42</t>
+  </si>
+  <si>
+    <t>케이팝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>태연</t>
+  </si>
+  <si>
+    <t>2b786fb3-a116-4163-9b65-cf56f03c8a7f</t>
+  </si>
+  <si>
+    <t>선미</t>
+  </si>
+  <si>
+    <t>716a8be4-6f58-4e64-a1e6-fb3017f21bf6</t>
+  </si>
+  <si>
+    <t>최예나</t>
+  </si>
+  <si>
+    <t>745c5b92-325f-451d-bd52-e6b95229c776</t>
+  </si>
+  <si>
+    <t>해외가수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RADWIMPS</t>
+  </si>
+  <si>
+    <t>해외가수</t>
+  </si>
+  <si>
+    <t>Coldplay</t>
+  </si>
+  <si>
+    <t>AJR</t>
+  </si>
+  <si>
+    <t>b1e26560-60e5-4236-bbdb-9aa5a8d5ee19</t>
+  </si>
+  <si>
+    <t>525f1f1c-03f0-4bc8-8dfd-e7521f87631b</t>
+  </si>
+  <si>
+    <t>5a85c140-dcf9-4dd2-b2c8-aff0471549f3</t>
+  </si>
+  <si>
+    <t>f4abc0b5-3f7a-4eff-8f78-ac078dbce533</t>
+  </si>
+  <si>
+    <t>b8a7c51f-362c-4dcb-a259-bc6e0095f0a6</t>
+  </si>
+  <si>
+    <t>afb680f2-b6eb-4cd7-a70b-a63b25c763d5</t>
+  </si>
+  <si>
+    <t>f4fdbb4c-e4b7-47a0-b83b-d91bbfcfa387</t>
+  </si>
+  <si>
+    <t>7eb1ce54-a355-41f9-8d68-e018b096d427</t>
+  </si>
+  <si>
+    <t>Lauv</t>
+  </si>
+  <si>
+    <t>YOASOBI</t>
+  </si>
+  <si>
+    <t>Anne-Marie</t>
+  </si>
+  <si>
+    <t>Eminem</t>
+  </si>
+  <si>
+    <t>Drake</t>
+  </si>
+  <si>
+    <t>Adele</t>
+  </si>
+  <si>
+    <t>에픽하이</t>
+  </si>
+  <si>
+    <t>힙합</t>
+  </si>
+  <si>
+    <t>싸이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f99b7d67-4e63-4678-aa66-4c6ac0f7d24a</t>
+  </si>
+  <si>
+    <t>힙합</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3dda8202-ce15-4031-862a-77bc6759d15e</t>
+  </si>
+  <si>
+    <t>로꼬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9e9e2a33-905c-4436-8ad8-8d9df00ba23d</t>
+  </si>
+  <si>
+    <t>6304678e-2d4b-4b1c-9f78-5444bace44b6</t>
+  </si>
+  <si>
+    <t>f2215143-d7db-4cf0-9cd4-b0040eb63cbd</t>
+  </si>
+  <si>
+    <t>d217c5ff-d768-49e1-ae32-3b1c5a3f5087</t>
+  </si>
+  <si>
+    <t>1b402bc8-aef9-4078-b3fd-ba3129b5daf8</t>
+  </si>
+  <si>
+    <t>비오</t>
+  </si>
+  <si>
+    <t>2228765c-f236-4db5-b576-cbad758dfc12</t>
+  </si>
+  <si>
+    <t>이영지</t>
+  </si>
+  <si>
+    <t>0433e75d-70b6-4118-9ff8-9b6f7e534093</t>
+  </si>
+  <si>
+    <t>비비</t>
+  </si>
+  <si>
+    <t>21c93d2d-dc10-4f8f-ae91-7285eff37c2f</t>
+  </si>
+  <si>
+    <t>제시</t>
+  </si>
+  <si>
+    <t>04b67fdc-8fdb-47e0-8307-d260abbc93f8</t>
+  </si>
+  <si>
+    <t>식케이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bbf6aa09-987b-46b6-8dd9-89c6ade3c00f</t>
+  </si>
+  <si>
+    <t>LANY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지코(ZICO)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>be465d46-9615-4722-b828-ea531ff97ea3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0d79fe8e-ba27-4859-bb8c-2f255f346853</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>48646387-1664-4c9a-9139-9bfd091b823c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>b9545342-1e6d-4dae-84ac-013374ad8d7c</t>
-  </si>
-  <si>
-    <t>인디</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>볼빨간사춘기</t>
-  </si>
-  <si>
-    <t>3529da27-3a5d-45bb-9308-4d131132a21e</t>
-  </si>
-  <si>
-    <t>백예린</t>
-  </si>
-  <si>
-    <t>d598652a-b64a-4e21-b607-bcec71698731</t>
-  </si>
-  <si>
-    <t>스텔라장</t>
-  </si>
-  <si>
-    <t>ece1a668-010c-4d2e-ad35-9985c950c320</t>
-  </si>
-  <si>
-    <t>헤이즈</t>
-  </si>
-  <si>
-    <t>8cea34d9-e1a5-4a92-87da-de947f741fe6</t>
-  </si>
-  <si>
-    <t>pH-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aace796b-0569-49b6-a144-64ea24031962 </t>
-  </si>
-  <si>
-    <t>투모로우바이투게더</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">9d027d72-790e-40ec-bbb7-61aa613457de </t>
-  </si>
-  <si>
-    <t>케이팝</t>
-  </si>
-  <si>
-    <t>세븐틴</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e04d239e-9fa8-49b3-b9b7-9e439c3cb1d1 </t>
-  </si>
-  <si>
-    <t>BTS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">0d79fe8e-ba27-4859-bb8c-2f255f346853 </t>
-  </si>
-  <si>
-    <t>NCT 127</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9d17d14a-e81c-410e-a90b-b02b0a9de6f8 </t>
-  </si>
-  <si>
-    <t>NCT DREAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dc7c8277-d4b6-4bca-bdfe-50eee42536ac </t>
-  </si>
-  <si>
-    <t>Stray Kids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">142b343d-bf5a-428c-a64f-6d1a7566bbe9 </t>
-  </si>
-  <si>
-    <t>몬스타엑스</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b6b21b0c-a706-4b46-a929-bd4d21b06cad </t>
-  </si>
-  <si>
-    <t>엔하이픈</t>
-  </si>
-  <si>
-    <t xml:space="preserve">95663592-1447-4579-90f7-c94733476667 </t>
-  </si>
-  <si>
-    <t>더보이즈</t>
-  </si>
-  <si>
-    <t xml:space="preserve">527973c7-9a9f-40bf-a52c-8cc2a7115c1a </t>
-  </si>
-  <si>
-    <t>SHINee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70e5098b-c4ae-4cd7-9799-3c1b9b57c753 </t>
-  </si>
-  <si>
-    <t>IVE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b2f2216a-d7a9-4ce0-8b8f-f494d9a8c196 </t>
-  </si>
-  <si>
-    <t>NewJeans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49204a7a-ed85-407a-828f-6fd46f1d8126 </t>
-  </si>
-  <si>
-    <t>(여자)아이들</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0068ae6c-7156-40f9-a81f-39294af6a549 </t>
-  </si>
-  <si>
-    <t>LE SSERAFIM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1ee37742-1e3d-4e61-84d2-bc85f4c1459a </t>
-  </si>
-  <si>
-    <t>aespa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b51c672b-85e0-48fe-8648-470a2422229f </t>
-  </si>
-  <si>
-    <t>STAYC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06bb5fcc-f2b3-428d-b8e7-079060311b6d </t>
-  </si>
-  <si>
-    <t>BLACKPINK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48646387-1664-4c9a-9139-9bfd091b823c </t>
-  </si>
-  <si>
-    <t>ITZY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bce172fc-51bb-43f7-9a25-b406a0a581d5 </t>
-  </si>
-  <si>
-    <t>TWICE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8da127cc-c432-418f-b356-ef36210d82ac </t>
-  </si>
-  <si>
-    <t>Red Velvet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4f0cb3b7-6c06-4317-ae35-ddf3106a17ee </t>
-  </si>
-  <si>
-    <t>NMIXX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2d623e82-73e2-4179-9c44-e963980f2d58 </t>
-  </si>
-  <si>
-    <t>마마무</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fb588f59-af1a-493a-9508-ed487caa2a11 </t>
-  </si>
-  <si>
-    <t>프로미스나인</t>
-  </si>
-  <si>
-    <t xml:space="preserve">705f04e2-fc5b-41ab-b837-1d850d44084a </t>
-  </si>
-  <si>
-    <t>WOODZ</t>
-  </si>
-  <si>
-    <t>25c73c37-9517-4144-8ef6-32541e82ff42</t>
-  </si>
-  <si>
-    <t>케이팝</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>태연</t>
-  </si>
-  <si>
-    <t>2b786fb3-a116-4163-9b65-cf56f03c8a7f</t>
-  </si>
-  <si>
-    <t>선미</t>
-  </si>
-  <si>
-    <t>716a8be4-6f58-4e64-a1e6-fb3017f21bf6</t>
-  </si>
-  <si>
-    <t>최예나</t>
-  </si>
-  <si>
-    <t>745c5b92-325f-451d-bd52-e6b95229c776</t>
-  </si>
-  <si>
-    <t>f1cc066a-6dd1-4b18-ae68-3708472ab4b1 </t>
-  </si>
-  <si>
-    <t>해외가수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Conan Gray</t>
-  </si>
-  <si>
-    <t>850a8b03-98a7-4fd3-afbd-5e5520b4ef5f </t>
-  </si>
-  <si>
-    <t>RADWIMPS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6f500293-7396-4903-b4fd-118127d06f9e </t>
-  </si>
-  <si>
-    <t>해외가수</t>
-  </si>
-  <si>
-    <t>Coldplay</t>
-  </si>
-  <si>
-    <t>cc197bad-dc9c-440d-a5b5-d52ba2e14234 </t>
-  </si>
-  <si>
-    <t>Imagine Dragons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">012151a8-0f9a-44c9-997f-ebd68b5389f9 </t>
-  </si>
-  <si>
-    <t>The 1975</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5b6ebfe0-f72b-4902-bba9-74c8af0f1af0 </t>
-  </si>
-  <si>
-    <t>Maroon 5</t>
-  </si>
-  <si>
-    <t>0ab49580-c84f-44d4-875f-d83760ea2cfe </t>
-  </si>
-  <si>
-    <t>AJR</t>
-  </si>
-  <si>
-    <t>2eb55bd9-cfbf-44fd-a5da-92dd825284c7 </t>
-  </si>
-  <si>
-    <t>Post Malone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b1e26560-60e5-4236-bbdb-9aa5a8d5ee19</t>
-  </si>
-  <si>
-    <t>Charlie Puth</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>525f1f1c-03f0-4bc8-8dfd-e7521f87631b</t>
-  </si>
-  <si>
-    <t>Sam Smith</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5a85c140-dcf9-4dd2-b2c8-aff0471549f3</t>
-  </si>
-  <si>
-    <t>Billie Eilish</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f4abc0b5-3f7a-4eff-8f78-ac078dbce533</t>
-  </si>
-  <si>
-    <t>Ed Sheeran</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b8a7c51f-362c-4dcb-a259-bc6e0095f0a6</t>
-  </si>
-  <si>
-    <t>Bruno Mars</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>afb680f2-b6eb-4cd7-a70b-a63b25c763d5</t>
-  </si>
-  <si>
-    <t>Ariana Grande</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f4fdbb4c-e4b7-47a0-b83b-d91bbfcfa387</t>
-  </si>
-  <si>
-    <t>Harry Styles</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7eb1ce54-a355-41f9-8d68-e018b096d427</t>
-  </si>
-  <si>
-    <t>Lauv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c0ef2ba5-a7b7-40ea-bd27-30acccfcac11 </t>
-  </si>
-  <si>
-    <t>The Kid LAROI</t>
-  </si>
-  <si>
-    <t>80609a00-b394-4a49-975b-2db6b543fa97 </t>
-  </si>
-  <si>
-    <t>b0337af1-8d93-4671-b6c9-ba306bf942bf </t>
-  </si>
-  <si>
-    <t>Taylor Swift</t>
-  </si>
-  <si>
-    <t>20244d07-534f-4eff-b4d4-930878889970 </t>
-  </si>
-  <si>
-    <t>YOASOBI</t>
-  </si>
-  <si>
-    <t>df6c619f-4334-43e2-8b6a-4a32af1e4f85 </t>
-  </si>
-  <si>
-    <t>Troye Sivan</t>
-  </si>
-  <si>
-    <t>e5712ceb-c37a-4c49-a11c-ccf4e21852d4 </t>
-  </si>
-  <si>
-    <t>Yonezu Kenshi</t>
-  </si>
-  <si>
-    <t>09d4a85c-4916-4b4e-bc96-c4cfcf371046 </t>
-  </si>
-  <si>
-    <t>The Weeknd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>c8b03190-306c-4120-bb0b-6f2ebfc06ea9 </t>
-  </si>
-  <si>
-    <t>Doja Cat</t>
-  </si>
-  <si>
-    <t>5df62a88-cac9-490a-b62c-c7c88f4020f4 </t>
-  </si>
-  <si>
-    <t>Anne-Marie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e3d5b5ec-101a-4529-9f2d-01dca64cf44e </t>
-  </si>
-  <si>
-    <t>Shawn Mendes</t>
-  </si>
-  <si>
-    <t>b7d92248-97e3-4450-8057-6fe06738f735 </t>
-  </si>
-  <si>
-    <t>Eminem</t>
-  </si>
-  <si>
-    <t>b95ce3ff-3d05-4e87-9e01-c97b66af13d4 </t>
-  </si>
-  <si>
-    <t>John K</t>
-  </si>
-  <si>
-    <t>be465d46-9615-4722-b828-ea531ff97ea3 </t>
-  </si>
-  <si>
-    <t>Drake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9fff2f8a-21e6-47de-a2b8-7f449929d43f </t>
-  </si>
-  <si>
-    <t>Dua Lipa</t>
-  </si>
-  <si>
-    <t>6f1a58bf-9b1b-49cf-a44a-6cefad7ae04f </t>
-  </si>
-  <si>
-    <t>Olivia Rodrigo</t>
-  </si>
-  <si>
-    <t>6925db17-f35e-42f3-a4eb-84ee6bf5d4b0 </t>
-  </si>
-  <si>
-    <t>Adele</t>
-  </si>
-  <si>
-    <t>cc2c9c3c-b7bc-4b8b-84d8-4fbd8779e493 </t>
-  </si>
-  <si>
-    <t>에픽하이</t>
-  </si>
-  <si>
-    <t xml:space="preserve">57f1cdd6-cf32-4004-a095-3ef043c91b61 </t>
-  </si>
-  <si>
-    <t>힙합</t>
-  </si>
-  <si>
-    <t>싸이</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f99b7d67-4e63-4678-aa66-4c6ac0f7d24a</t>
-  </si>
-  <si>
-    <t>힙합</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3dda8202-ce15-4031-862a-77bc6759d15e</t>
-  </si>
-  <si>
-    <t>로꼬</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>9e9e2a33-905c-4436-8ad8-8d9df00ba23d</t>
-  </si>
-  <si>
-    <t>사이먼 도미닉</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6304678e-2d4b-4b1c-9f78-5444bace44b6</t>
-  </si>
-  <si>
-    <t>지코</t>
-  </si>
-  <si>
-    <t>f2215143-d7db-4cf0-9cd4-b0040eb63cbd</t>
-  </si>
-  <si>
-    <t>Young K</t>
-  </si>
-  <si>
-    <t>d217c5ff-d768-49e1-ae32-3b1c5a3f5087</t>
-  </si>
-  <si>
-    <t>Ash Island</t>
-  </si>
-  <si>
-    <t>1b402bc8-aef9-4078-b3fd-ba3129b5daf8</t>
-  </si>
-  <si>
-    <t>비오</t>
-  </si>
-  <si>
-    <t>2228765c-f236-4db5-b576-cbad758dfc12</t>
-  </si>
-  <si>
-    <t>이영지</t>
-  </si>
-  <si>
-    <t>0433e75d-70b6-4118-9ff8-9b6f7e534093</t>
-  </si>
-  <si>
-    <t>비비</t>
-  </si>
-  <si>
-    <t>21c93d2d-dc10-4f8f-ae91-7285eff37c2f</t>
-  </si>
-  <si>
-    <t>제시</t>
-  </si>
-  <si>
-    <t>04b67fdc-8fdb-47e0-8307-d260abbc93f8</t>
-  </si>
-  <si>
-    <t>식케이</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bbf6aa09-987b-46b6-8dd9-89c6ade3c00f</t>
-  </si>
-  <si>
-    <t>Central Cee</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jay Park</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LANY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dc7c8277-d4b6-4bca-bdfe-50eee42536ac</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NCTDREAM</t>
+  </si>
+  <si>
+    <t>49204a7a-ed85-407a-828f-6fd46f1d8126</t>
+  </si>
+  <si>
+    <t>b2f2216a-d7a9-4ce0-8b8f-f494d9a8c196</t>
+  </si>
+  <si>
+    <t>JayPark</t>
+  </si>
+  <si>
+    <t>9d027d72-790e-40ec-bbb7-61aa613457de</t>
+  </si>
+  <si>
+    <t>e04d239e-9fa8-49b3-b9b7-9e439c3cb1d1</t>
+  </si>
+  <si>
+    <t>NCT127</t>
+  </si>
+  <si>
+    <t>9d17d14a-e81c-410e-a90b-b02b0a9de6f8</t>
+  </si>
+  <si>
+    <t>StrayKids</t>
+  </si>
+  <si>
+    <t>142b343d-bf5a-428c-a64f-6d1a7566bbe9</t>
+  </si>
+  <si>
+    <t>PostMalone</t>
+  </si>
+  <si>
+    <t>CharliePuth</t>
+  </si>
+  <si>
+    <t>TaylorSwift</t>
+  </si>
+  <si>
+    <t>20244d07-534f-4eff-b4d4-930878889970</t>
+  </si>
+  <si>
+    <t>SamSmith</t>
+  </si>
+  <si>
+    <t>e156615d-3ddd-4491-9584-4b9d971472c4</t>
+  </si>
+  <si>
+    <t>77191d5f-1045-4b3b-ad7f-12ea398db929</t>
+  </si>
+  <si>
+    <t>730182f9-2b25-45cc-857a-054c2bbe8ade</t>
+  </si>
+  <si>
+    <t>사이먼도미닉</t>
+  </si>
+  <si>
+    <t>f619b92a-a1b5-481c-8405-df35fb7846f1</t>
+  </si>
+  <si>
+    <t>a697464c-69b1-4bbc-88cc-570c025a25e5</t>
+  </si>
+  <si>
+    <t>ArianaGrande</t>
+  </si>
+  <si>
+    <t>HarryStyles</t>
+  </si>
+  <si>
+    <t>c0ef2ba5-a7b7-40ea-bd27-30acccfcac11</t>
+  </si>
+  <si>
+    <t>57f1cdd6-cf32-4004-a095-3ef043c91b61</t>
+  </si>
+  <si>
+    <t>wavetoearth</t>
+  </si>
+  <si>
+    <t>89e95aa3-bd49-4af3-9c87-0d88b2093bb0</t>
+  </si>
+  <si>
+    <t>TheKidLAROI</t>
+  </si>
+  <si>
+    <t>80609a00-b394-4a49-975b-2db6b543fa97</t>
+  </si>
+  <si>
+    <t>b6b21b0c-a706-4b46-a929-bd4d21b06cad</t>
+  </si>
+  <si>
+    <t>95663592-1447-4579-90f7-c94733476667</t>
+  </si>
+  <si>
+    <t>527973c7-9a9f-40bf-a52c-8cc2a7115c1a</t>
+  </si>
+  <si>
+    <t>70e5098b-c4ae-4cd7-9799-3c1b9b57c753</t>
+  </si>
+  <si>
+    <t>0068ae6c-7156-40f9-a81f-39294af6a549</t>
+  </si>
+  <si>
+    <t>LESSERAFIM</t>
+  </si>
+  <si>
+    <t>1ee37742-1e3d-4e61-84d2-bc85f4c1459a</t>
+  </si>
+  <si>
+    <t>b51c672b-85e0-48fe-8648-470a2422229f</t>
+  </si>
+  <si>
+    <t>06bb5fcc-f2b3-428d-b8e7-079060311b6d</t>
+  </si>
+  <si>
+    <t>PaulKim</t>
+  </si>
+  <si>
+    <t>bce172fc-51bb-43f7-9a25-b406a0a581d5</t>
+  </si>
+  <si>
+    <t>8da127cc-c432-418f-b356-ef36210d82ac</t>
+  </si>
+  <si>
+    <t>RedVelvet</t>
+  </si>
+  <si>
+    <t>4f0cb3b7-6c06-4317-ae35-ddf3106a17ee</t>
+  </si>
+  <si>
+    <t>2d623e82-73e2-4179-9c44-e963980f2d58</t>
+  </si>
+  <si>
+    <t>fb588f59-af1a-493a-9508-ed487caa2a11</t>
+  </si>
+  <si>
+    <t>프로미스나인(Promise9)</t>
+  </si>
+  <si>
+    <t>705f04e2-fc5b-41ab-b837-1d850d44084a</t>
+  </si>
+  <si>
+    <t>f1cc066a-6dd1-4b18-ae68-3708472ab4b1</t>
+  </si>
+  <si>
+    <t>ConanGray</t>
+  </si>
+  <si>
+    <t>850a8b03-98a7-4fd3-afbd-5e5520b4ef5f</t>
+  </si>
+  <si>
+    <t>6f500293-7396-4903-b4fd-118127d06f9e</t>
+  </si>
+  <si>
+    <t>cc197bad-dc9c-440d-a5b5-d52ba2e14234</t>
+  </si>
+  <si>
+    <t>ImagineDragons</t>
+  </si>
+  <si>
+    <t>012151a8-0f9a-44c9-997f-ebd68b5389f9</t>
+  </si>
+  <si>
+    <t>Maroon5</t>
+  </si>
+  <si>
+    <t>0ab49580-c84f-44d4-875f-d83760ea2cfe</t>
+  </si>
+  <si>
+    <t>2eb55bd9-cfbf-44fd-a5da-92dd825284c7</t>
+  </si>
+  <si>
+    <t>dea836e0-66dd-4285-9cab-2272bcda93b8</t>
+  </si>
+  <si>
+    <t>BillieEilish</t>
+  </si>
+  <si>
+    <t>EdSheeran</t>
+  </si>
+  <si>
+    <t>BrunoMars</t>
+  </si>
+  <si>
+    <t>TroyeSivan</t>
+  </si>
+  <si>
+    <t>e5712ceb-c37a-4c49-a11c-ccf4e21852d4</t>
+  </si>
+  <si>
+    <t>YonezuKenshi</t>
+  </si>
+  <si>
+    <t>09d4a85c-4916-4b4e-bc96-c4cfcf371046</t>
+  </si>
+  <si>
+    <t>TheWeeknd</t>
+  </si>
+  <si>
+    <t>c8b03190-306c-4120-bb0b-6f2ebfc06ea9</t>
+  </si>
+  <si>
+    <t>CentralCee</t>
+  </si>
+  <si>
+    <t>b0337af1-8d93-4671-b6c9-ba306bf942bf</t>
+  </si>
+  <si>
+    <t>df6c619f-4334-43e2-8b6a-4a32af1e4f85</t>
+  </si>
+  <si>
+    <t>DojaCat</t>
+  </si>
+  <si>
+    <t>5df62a88-cac9-490a-b62c-c7c88f4020f4</t>
+  </si>
+  <si>
+    <t>e3d5b5ec-101a-4529-9f2d-01dca64cf44e</t>
+  </si>
+  <si>
+    <t>ShawnMendes</t>
+  </si>
+  <si>
+    <t>b7d92248-97e3-4450-8057-6fe06738f735</t>
+  </si>
+  <si>
+    <t>b95ce3ff-3d05-4e87-9e01-c97b66af13d4</t>
+  </si>
+  <si>
+    <t>JohnK</t>
+  </si>
+  <si>
+    <t>9fff2f8a-21e6-47de-a2b8-7f449929d43f</t>
+  </si>
+  <si>
+    <t>DuaLipa</t>
+  </si>
+  <si>
+    <t>6f1a58bf-9b1b-49cf-a44a-6cefad7ae04f</t>
+  </si>
+  <si>
+    <t>OliviaRodrigo</t>
+  </si>
+  <si>
+    <t>6925db17-f35e-42f3-a4eb-84ee6bf5d4b0</t>
+  </si>
+  <si>
+    <t>cc2c9c3c-b7bc-4b8b-84d8-4fbd8779e493</t>
+  </si>
+  <si>
+    <t>aace796b-0569-49b6-a144-64ea24031962</t>
+  </si>
+  <si>
+    <t>YoungK</t>
+  </si>
+  <si>
+    <t>AshIsland</t>
   </si>
 </sst>
 </file>
@@ -1124,10 +1112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A18E46-C40A-D44C-92D2-00EB00D6AF41}">
-  <dimension ref="A1:E128"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="17.25" customHeight="1"/>
@@ -1140,196 +1128,196 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20">
       <c r="A1" s="2" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="C1" s="4">
         <v>70113</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" ht="20">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
       <c r="C2" s="4">
         <v>987404</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="20">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="C3" s="4">
         <v>264991</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" ht="20">
       <c r="A4" s="2" t="s">
-        <v>62</v>
+        <v>117</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="C4" s="4">
         <v>994221</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="20">
       <c r="A5" s="2" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="C5" s="4">
         <v>3239944</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="18">
       <c r="A6" s="2" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="C6" s="8">
         <v>2937324</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="20">
       <c r="A7" s="2" t="s">
-        <v>203</v>
+        <v>120</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>181</v>
+        <v>93</v>
       </c>
       <c r="C7" s="4">
         <v>11593</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>180</v>
+        <v>92</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" ht="20">
       <c r="A8" s="6" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>54</v>
+        <v>121</v>
       </c>
       <c r="C8" s="4">
         <v>1692196</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="20">
       <c r="A9" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>57</v>
+        <v>122</v>
       </c>
       <c r="C9" s="4">
         <v>961718</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" ht="20">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C10" s="4">
         <v>2382659</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="20">
       <c r="A11" s="2" t="s">
-        <v>60</v>
+        <v>123</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="C11" s="4">
         <v>970192</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="20">
       <c r="A12" s="2" t="s">
-        <v>64</v>
+        <v>125</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
       <c r="C12" s="4">
         <v>1233909</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="20">
       <c r="A13" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>127</v>
+        <v>74</v>
       </c>
       <c r="C13" s="4">
         <v>326362</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="E13" s="2"/>
     </row>
@@ -1338,208 +1326,208 @@
         <v>128</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>129</v>
+        <v>75</v>
       </c>
       <c r="C14" s="4">
         <v>250301</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" ht="20">
       <c r="A15" s="2" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="C15" s="4">
         <v>1177</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="20">
       <c r="A16" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>131</v>
+        <v>76</v>
       </c>
       <c r="C16" s="4">
         <v>43383</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" ht="20">
       <c r="A17" s="2" t="s">
-        <v>178</v>
+        <v>90</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>179</v>
+        <v>91</v>
       </c>
       <c r="C17" s="4">
         <v>24364</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>180</v>
+        <v>92</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" ht="20">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>17</v>
+        <v>132</v>
       </c>
       <c r="C18" s="4">
         <v>1302105</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" ht="20">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="C19" s="4">
         <v>893747</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" ht="20">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>22</v>
+        <v>134</v>
       </c>
       <c r="C20" s="4">
         <v>1509383</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="20">
       <c r="A21" s="2" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
       <c r="C21" s="4">
         <v>39141</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>180</v>
+        <v>92</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="20">
       <c r="A22" s="2" t="s">
-        <v>184</v>
+        <v>135</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>185</v>
+        <v>96</v>
       </c>
       <c r="C22" s="4">
         <v>297553</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>180</v>
+        <v>92</v>
       </c>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" ht="20">
       <c r="A23" s="2" t="s">
-        <v>186</v>
+        <v>111</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>187</v>
+        <v>97</v>
       </c>
       <c r="C23" s="4">
         <v>217593</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>180</v>
+        <v>92</v>
       </c>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" ht="20">
       <c r="A24" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C24" s="4">
         <v>845618</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" ht="20">
       <c r="A25" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>36</v>
+        <v>136</v>
       </c>
       <c r="C25" s="4">
         <v>318857</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" ht="20">
       <c r="A26" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>39</v>
+        <v>137</v>
       </c>
       <c r="C26" s="4">
         <v>980734</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" ht="20">
       <c r="A27" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C27" s="4">
         <v>1010174</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E27" s="2"/>
     </row>
@@ -1548,88 +1536,88 @@
         <v>138</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>139</v>
+        <v>80</v>
       </c>
       <c r="C28" s="4">
         <v>26507</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" ht="20">
       <c r="A29" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>141</v>
+        <v>81</v>
       </c>
       <c r="C29" s="4">
         <v>22457</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" ht="20">
       <c r="A30" s="2" t="s">
-        <v>142</v>
+        <v>82</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C30" s="4">
         <v>338777</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" ht="20">
       <c r="A31" s="2" t="s">
-        <v>175</v>
+        <v>88</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="C31" s="4">
         <v>12024</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>177</v>
+        <v>89</v>
       </c>
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" ht="20">
       <c r="A32" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C32" s="4">
         <v>1491178</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" ht="20">
       <c r="A33" s="2" t="s">
-        <v>33</v>
+        <v>142</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>34</v>
+        <v>143</v>
       </c>
       <c r="C33" s="4">
         <v>2894691</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E33" s="2"/>
     </row>
@@ -1649,10 +1637,10 @@
     </row>
     <row r="35" spans="1:5" ht="20">
       <c r="A35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="C35" s="4">
         <v>245350</v>
@@ -1663,10 +1651,10 @@
     </row>
     <row r="36" spans="1:5" ht="20">
       <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="C36" s="4">
         <v>21408</v>
@@ -1686,129 +1674,129 @@
         <v>1546645</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="20">
       <c r="A38" s="2" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>67</v>
+        <v>146</v>
       </c>
       <c r="C38" s="4">
         <v>653084</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="20">
       <c r="A39" s="2" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>69</v>
+        <v>147</v>
       </c>
       <c r="C39" s="4">
         <v>2406628</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5" ht="20">
       <c r="A40" s="2" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>71</v>
+        <v>148</v>
       </c>
       <c r="C40" s="4">
         <v>6429</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E40" s="1"/>
     </row>
     <row r="41" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A41" s="2" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>73</v>
+        <v>149</v>
       </c>
       <c r="C41" s="4">
         <v>183121</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A42" s="2" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>79</v>
+        <v>150</v>
       </c>
       <c r="C42" s="4">
         <v>1458475</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A43" s="2" t="s">
-        <v>80</v>
+        <v>151</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>81</v>
+        <v>152</v>
       </c>
       <c r="C43" s="4">
         <v>3109717</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A44" s="2" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>83</v>
+        <v>153</v>
       </c>
       <c r="C44" s="4">
         <v>2449018</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A45" s="2" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>85</v>
+        <v>154</v>
       </c>
       <c r="C45" s="4">
         <v>2464445</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A46" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="C46" s="4">
         <v>96797</v>
@@ -1819,766 +1807,755 @@
     </row>
     <row r="47" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A47" s="2" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>89</v>
+        <v>156</v>
       </c>
       <c r="C47" s="4">
         <v>1703914</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A48" s="2" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="C48" s="4">
         <v>211474</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A49" s="2" t="s">
-        <v>92</v>
+        <v>158</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>93</v>
+        <v>159</v>
       </c>
       <c r="C49" s="4">
         <v>457228</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A50" s="2" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>95</v>
+        <v>160</v>
       </c>
       <c r="C50" s="4">
         <v>3035769</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E50" s="2"/>
     </row>
     <row r="51" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A51" s="2" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>97</v>
+        <v>161</v>
       </c>
       <c r="C51" s="4">
         <v>559263</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A52" s="2" t="s">
-        <v>98</v>
+        <v>162</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>99</v>
+        <v>163</v>
       </c>
       <c r="C52" s="4">
         <v>1487923</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A53" s="2" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="C53" s="4">
         <v>1378784</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A54" s="2" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="C54" s="4">
         <v>405774</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E54"/>
     </row>
     <row r="55" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A55" s="2" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="C55" s="4">
         <v>623218</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="E55"/>
     </row>
     <row r="56" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A56" s="2" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="C56" s="4">
         <v>2304606</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A57" s="2" t="s">
-        <v>204</v>
+        <v>110</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>109</v>
+        <v>164</v>
       </c>
       <c r="C57" s="4">
         <v>247886</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A58" s="2" t="s">
-        <v>111</v>
+        <v>165</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>112</v>
+        <v>166</v>
       </c>
       <c r="C58" s="4">
         <v>621686</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A59" s="2" t="s">
-        <v>113</v>
+        <v>70</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>114</v>
+        <v>167</v>
       </c>
       <c r="C59" s="4">
         <v>383998</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A60" s="2" t="s">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>117</v>
+        <v>168</v>
       </c>
       <c r="C60" s="4">
         <v>8351</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A61" s="2" t="s">
-        <v>118</v>
+        <v>169</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>119</v>
+        <v>170</v>
       </c>
       <c r="C61" s="4">
         <v>29472</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A62" s="2" t="s">
-        <v>120</v>
+        <v>171</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>121</v>
+        <v>172</v>
       </c>
       <c r="C62" s="4">
-        <v>45824</v>
+        <v>13539</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A63" s="2" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>123</v>
+        <v>173</v>
       </c>
       <c r="C63" s="4">
-        <v>13539</v>
+        <v>164661</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A64" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>125</v>
+        <v>10</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C64" s="4">
-        <v>164661</v>
+        <v>1056920</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>115</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A65" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B65" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="B65" s="5" t="s">
+        <v>174</v>
+      </c>
       <c r="C65" s="4">
-        <v>1056920</v>
+        <v>381732</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A66" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C66" s="4">
-        <v>381732</v>
+        <v>1820763</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A67" s="2" t="s">
-        <v>9</v>
+        <v>175</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="C67" s="4">
-        <v>1820763</v>
+        <v>615550</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A68" s="2" t="s">
-        <v>132</v>
+        <v>176</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>133</v>
+        <v>78</v>
       </c>
       <c r="C68" s="4">
-        <v>615550</v>
+        <v>12418</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A69" s="2" t="s">
-        <v>134</v>
+        <v>177</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>135</v>
+        <v>79</v>
       </c>
       <c r="C69" s="4">
-        <v>12418</v>
+        <v>500</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="70" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A70" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>137</v>
+        <v>178</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>179</v>
       </c>
       <c r="C70" s="4">
-        <v>500</v>
+        <v>161507</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A71" s="2" t="s">
-        <v>151</v>
+        <v>180</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>152</v>
+        <v>181</v>
       </c>
       <c r="C71" s="4">
-        <v>161507</v>
+        <v>1090113</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A72" s="2" t="s">
-        <v>153</v>
+        <v>182</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>154</v>
+        <v>183</v>
       </c>
       <c r="C72" s="4">
-        <v>1090113</v>
+        <v>2358</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A73" s="2" t="s">
-        <v>155</v>
+        <v>184</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>156</v>
+        <v>185</v>
       </c>
       <c r="C73" s="4">
-        <v>2358</v>
+        <v>897106</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A74" s="2" t="s">
-        <v>202</v>
+        <v>83</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="C74" s="4">
-        <v>897106</v>
+        <v>2270044</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A75" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>150</v>
+        <v>104</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="C75" s="4">
-        <v>2270044</v>
+        <v>1825718</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
     </row>
     <row r="76" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A76" s="2" t="s">
-        <v>196</v>
+        <v>106</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>197</v>
+        <v>107</v>
       </c>
       <c r="C76" s="4">
-        <v>1825718</v>
+        <v>672794</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>180</v>
+        <v>92</v>
       </c>
     </row>
     <row r="77" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A77" s="2" t="s">
-        <v>198</v>
+        <v>108</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>199</v>
+        <v>109</v>
       </c>
       <c r="C77" s="4">
-        <v>672794</v>
+        <v>988518</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>180</v>
+        <v>92</v>
       </c>
     </row>
     <row r="78" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A78" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>201</v>
+        <v>187</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>188</v>
       </c>
       <c r="C78" s="4">
-        <v>988518</v>
+        <v>139478</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>180</v>
+        <v>69</v>
       </c>
     </row>
     <row r="79" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A79" s="2" t="s">
-        <v>157</v>
+        <v>84</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>158</v>
+        <v>189</v>
       </c>
       <c r="C79" s="4">
-        <v>139478</v>
+        <v>296675</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="80" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A80" s="2" t="s">
-        <v>159</v>
+        <v>190</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>160</v>
+        <v>191</v>
       </c>
       <c r="C80" s="4">
-        <v>296675</v>
+        <v>195029</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="81" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A81" s="2" t="s">
-        <v>161</v>
+        <v>85</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>162</v>
+        <v>192</v>
       </c>
       <c r="C81" s="4">
-        <v>195029</v>
+        <v>45</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A82" s="2" t="s">
-        <v>163</v>
+        <v>193</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>164</v>
+        <v>112</v>
       </c>
       <c r="C82" s="4">
-        <v>45</v>
+        <v>1219340</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A83" s="2" t="s">
-        <v>165</v>
+        <v>86</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
       <c r="C83" s="4">
-        <v>1219340</v>
+        <v>130</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A84" s="2" t="s">
-        <v>167</v>
+        <v>195</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="C84" s="4">
-        <v>130</v>
+        <v>555561</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A85" s="2" t="s">
-        <v>169</v>
+        <v>197</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="C85" s="4">
-        <v>555561</v>
+        <v>1599675</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="86" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A86" s="2" t="s">
-        <v>171</v>
+        <v>87</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>172</v>
+        <v>199</v>
       </c>
       <c r="C86" s="4">
-        <v>1599675</v>
+        <v>2300</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="87" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A87" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>174</v>
+        <v>37</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="C87" s="4">
-        <v>2300</v>
+        <v>1139312</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>110</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E87" s="2"/>
     </row>
     <row r="88" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A88" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C88" s="4">
-        <v>1139312</v>
+        <v>116155</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E88" s="2"/>
+        <v>32</v>
+      </c>
     </row>
     <row r="89" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A89" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="C89" s="4">
-        <v>116155</v>
+        <v>1008975</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
     </row>
     <row r="90" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A90" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>52</v>
+        <v>201</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="C90" s="4">
-        <v>1008975</v>
+        <v>11864</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>180</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A91" s="2" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>189</v>
+        <v>99</v>
       </c>
       <c r="C91" s="4">
-        <v>11864</v>
+        <v>1639884</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A92" s="2" t="s">
-        <v>190</v>
+        <v>100</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>191</v>
+        <v>101</v>
       </c>
       <c r="C92" s="4">
-        <v>1639884</v>
+        <v>2043567</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>180</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E92" s="2"/>
     </row>
     <row r="93" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A93" s="2" t="s">
-        <v>192</v>
+        <v>102</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>193</v>
+        <v>103</v>
       </c>
       <c r="C93" s="4">
-        <v>2043567</v>
+        <v>1767632</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E93" s="2"/>
+        <v>92</v>
+      </c>
     </row>
     <row r="94" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A94" s="2" t="s">
-        <v>194</v>
+        <v>18</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>195</v>
+        <v>19</v>
       </c>
       <c r="C94" s="4">
-        <v>1767632</v>
+        <v>1075500</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>180</v>
+        <v>16</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A95" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C95" s="4">
-        <v>1075500</v>
+        <v>986023</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A96" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C96" s="4">
-        <v>986023</v>
+        <v>358775</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" s="1" customFormat="1" ht="20">
-      <c r="A97" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C97" s="4">
-        <v>358775</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" s="1" customFormat="1" ht="18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" s="1" customFormat="1" ht="18">
+      <c r="B97"/>
+    </row>
+    <row r="98" spans="2:2" s="1" customFormat="1" ht="18">
       <c r="B98"/>
     </row>
-    <row r="99" spans="1:4" s="1" customFormat="1" ht="18">
+    <row r="99" spans="2:2" s="1" customFormat="1" ht="18">
       <c r="B99"/>
     </row>
-    <row r="100" spans="1:4" s="1" customFormat="1" ht="18">
+    <row r="100" spans="2:2" s="1" customFormat="1" ht="18">
       <c r="B100"/>
     </row>
-    <row r="101" spans="1:4" s="1" customFormat="1" ht="18">
+    <row r="101" spans="2:2" s="1" customFormat="1" ht="18">
       <c r="B101"/>
     </row>
-    <row r="102" spans="1:4" s="1" customFormat="1" ht="18">
+    <row r="102" spans="2:2" s="1" customFormat="1" ht="18">
       <c r="B102"/>
     </row>
-    <row r="103" spans="1:4" s="1" customFormat="1" ht="18">
+    <row r="103" spans="2:2" s="1" customFormat="1" ht="18">
       <c r="B103"/>
     </row>
-    <row r="104" spans="1:4" s="1" customFormat="1" ht="18">
+    <row r="104" spans="2:2" s="1" customFormat="1" ht="18">
       <c r="B104"/>
     </row>
-    <row r="105" spans="1:4" s="1" customFormat="1" ht="18">
+    <row r="105" spans="2:2" s="1" customFormat="1" ht="18">
       <c r="B105"/>
     </row>
-    <row r="106" spans="1:4" s="1" customFormat="1" ht="18">
+    <row r="106" spans="2:2" s="1" customFormat="1" ht="18">
       <c r="B106"/>
     </row>
-    <row r="107" spans="1:4" s="1" customFormat="1" ht="18">
+    <row r="107" spans="2:2" s="1" customFormat="1" ht="18">
       <c r="B107"/>
     </row>
-    <row r="108" spans="1:4" s="1" customFormat="1" ht="18">
+    <row r="108" spans="2:2" s="1" customFormat="1" ht="18">
       <c r="B108"/>
     </row>
-    <row r="109" spans="1:4" s="1" customFormat="1" ht="18">
+    <row r="109" spans="2:2" s="1" customFormat="1" ht="18">
       <c r="B109"/>
     </row>
-    <row r="110" spans="1:4" s="1" customFormat="1" ht="18">
+    <row r="110" spans="2:2" s="1" customFormat="1" ht="18">
       <c r="B110"/>
     </row>
-    <row r="111" spans="1:4" s="1" customFormat="1" ht="18">
+    <row r="111" spans="2:2" s="1" customFormat="1" ht="18">
       <c r="B111"/>
     </row>
-    <row r="112" spans="1:4" s="1" customFormat="1" ht="18">
+    <row r="112" spans="2:2" s="1" customFormat="1" ht="18">
       <c r="B112"/>
     </row>
     <row r="113" spans="2:2" s="1" customFormat="1" ht="18">
@@ -2626,12 +2603,9 @@
     <row r="127" spans="2:2" s="1" customFormat="1" ht="18">
       <c r="B127"/>
     </row>
-    <row r="128" spans="2:2" s="1" customFormat="1" ht="18">
-      <c r="B128"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E94">
-    <sortCondition ref="D1:D94"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E93">
+    <sortCondition ref="D1:D93"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Fix] onboardingView button disable
</commit_message>
<xml_diff>
--- a/Projects/App/Resources/onboardingArtist.xlsx
+++ b/Projects/App/Resources/onboardingArtist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choihyowon/Desktop/2023/ADA/Mac/Setlist/Projects/App/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7316B464-BCEE-BA4F-83AB-C9BDF90643A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB658EA-6D11-BF42-9030-B6E06DC98FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15640" xr2:uid="{DDFC3EF1-0C9B-2449-839F-441E442BC4BA}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="장르별 30명씩" sheetId="9" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'장르별 30명씩'!$A$18:$D$126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'장르별 30명씩'!$A$17:$D$124</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="199">
   <si>
     <t>카더가든</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -154,15 +154,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>볼빨간사춘기</t>
-  </si>
-  <si>
-    <t>3529da27-3a5d-45bb-9308-4d131132a21e</t>
-  </si>
-  <si>
-    <t>백예린</t>
-  </si>
-  <si>
     <t>d598652a-b64a-4e21-b607-bcec71698731</t>
   </si>
   <si>
@@ -207,9 +198,6 @@
     <t>SHINee</t>
   </si>
   <si>
-    <t>IVE</t>
-  </si>
-  <si>
     <t>NewJeans</t>
   </si>
   <si>
@@ -380,10 +368,6 @@
     <t>04b67fdc-8fdb-47e0-8307-d260abbc93f8</t>
   </si>
   <si>
-    <t>식케이</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>bbf6aa09-987b-46b6-8dd9-89c6ade3c00f</t>
   </si>
   <si>
@@ -421,9 +405,6 @@
     <t>49204a7a-ed85-407a-828f-6fd46f1d8126</t>
   </si>
   <si>
-    <t>b2f2216a-d7a9-4ce0-8b8f-f494d9a8c196</t>
-  </si>
-  <si>
     <t>JayPark</t>
   </si>
   <si>
@@ -547,9 +528,6 @@
     <t>fb588f59-af1a-493a-9508-ed487caa2a11</t>
   </si>
   <si>
-    <t>프로미스나인(Promise9)</t>
-  </si>
-  <si>
     <t>705f04e2-fc5b-41ab-b837-1d850d44084a</t>
   </si>
   <si>
@@ -679,6 +657,18 @@
   </si>
   <si>
     <t>77191d5f-1045-4b3b-ad7f-12ea398db929</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yerin Baek</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로미스나인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sik-k</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -686,7 +676,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -738,14 +728,6 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -772,7 +754,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -795,9 +777,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1115,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A18E46-C40A-D44C-92D2-00EB00D6AF41}">
-  <dimension ref="A1:E127"/>
+  <dimension ref="A1:E125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="17.25" customHeight="1"/>
@@ -1131,31 +1110,31 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C1" s="4">
         <v>70113</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" ht="20">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C2" s="4">
         <v>987404</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -1164,7 +1143,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C3" s="4">
         <v>264991</v>
@@ -1176,238 +1155,238 @@
     </row>
     <row r="4" spans="1:5" ht="20">
       <c r="A4" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C4" s="4">
         <v>994221</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="20">
       <c r="A5" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C5" s="4">
         <v>3239944</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="18">
+    <row r="6" spans="1:5" ht="20">
       <c r="A6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" s="8">
-        <v>2937324</v>
+        <v>112</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="4">
+        <v>11593</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="20">
-      <c r="A7" s="2" t="s">
-        <v>118</v>
+      <c r="A7" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="C7" s="4">
-        <v>11593</v>
+        <v>1692196</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" ht="20">
-      <c r="A8" s="6" t="s">
-        <v>42</v>
+      <c r="A8" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C8" s="4">
-        <v>1692196</v>
+        <v>961718</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="20">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>120</v>
+        <v>25</v>
       </c>
       <c r="C9" s="4">
-        <v>961718</v>
+        <v>2382659</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" ht="20">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>116</v>
       </c>
       <c r="C10" s="4">
-        <v>2382659</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>16</v>
+        <v>970192</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="20">
       <c r="A11" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C11" s="4">
-        <v>970192</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>43</v>
+        <v>1233909</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="20">
       <c r="A12" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>124</v>
+        <v>70</v>
       </c>
       <c r="C12" s="4">
-        <v>1233909</v>
+        <v>326362</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="20">
       <c r="A13" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>74</v>
+        <v>193</v>
       </c>
       <c r="C13" s="4">
-        <v>326362</v>
+        <v>250301</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" ht="20">
       <c r="A14" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>200</v>
+        <v>121</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>122</v>
       </c>
       <c r="C14" s="4">
-        <v>250301</v>
+        <v>1177</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" ht="20">
       <c r="A15" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C15" s="4">
-        <v>1177</v>
+        <v>43383</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="20">
       <c r="A16" s="2" t="s">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>75</v>
+        <v>194</v>
       </c>
       <c r="C16" s="4">
-        <v>43383</v>
+        <v>24364</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" ht="20">
       <c r="A17" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>201</v>
+        <v>14</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="C17" s="4">
-        <v>24364</v>
+        <v>1302105</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>90</v>
+        <v>13</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" ht="20">
       <c r="A18" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>130</v>
+        <v>195</v>
       </c>
       <c r="C18" s="4">
-        <v>1302105</v>
+        <v>893747</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" ht="20">
       <c r="A19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>202</v>
+        <v>17</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="C19" s="4">
-        <v>893747</v>
+        <v>1509383</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>16</v>
@@ -1416,88 +1395,88 @@
     </row>
     <row r="20" spans="1:5" ht="20">
       <c r="A20" s="2" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>131</v>
+        <v>89</v>
       </c>
       <c r="C20" s="4">
-        <v>1509383</v>
+        <v>39141</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="20">
       <c r="A21" s="2" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C21" s="4">
-        <v>39141</v>
+        <v>297553</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="20">
       <c r="A22" s="2" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C22" s="4">
-        <v>297553</v>
+        <v>217593</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" ht="20">
       <c r="A23" s="2" t="s">
-        <v>109</v>
+        <v>196</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>95</v>
+        <v>33</v>
       </c>
       <c r="C23" s="4">
-        <v>217593</v>
+        <v>845618</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>90</v>
+        <v>32</v>
       </c>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" ht="20">
       <c r="A24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>127</v>
       </c>
       <c r="C24" s="4">
-        <v>845618</v>
+        <v>318857</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" ht="20">
       <c r="A25" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C25" s="4">
-        <v>318857</v>
+        <v>980734</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>29</v>
@@ -1506,133 +1485,131 @@
     </row>
     <row r="26" spans="1:5" ht="20">
       <c r="A26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="C26" s="4">
-        <v>980734</v>
+        <v>26507</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" ht="20">
       <c r="A27" s="2" t="s">
-        <v>33</v>
+        <v>130</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="C27" s="4">
-        <v>1010174</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>29</v>
+        <v>22457</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" ht="20">
       <c r="A28" s="2" t="s">
-        <v>135</v>
+        <v>77</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>79</v>
+        <v>131</v>
       </c>
       <c r="C28" s="4">
-        <v>26507</v>
+        <v>338777</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" ht="20">
       <c r="A29" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="C29" s="4">
-        <v>22457</v>
+        <v>12024</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" ht="20">
       <c r="A30" s="2" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>137</v>
+        <v>27</v>
       </c>
       <c r="C30" s="4">
-        <v>338777</v>
+        <v>1491178</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" ht="20">
       <c r="A31" s="2" t="s">
-        <v>87</v>
+        <v>133</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C31" s="4">
-        <v>12024</v>
+        <v>2894691</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" ht="20">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C32" s="4">
-        <v>1491178</v>
+        <v>1093913</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="2"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="33" spans="1:5" ht="20">
       <c r="A33" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>140</v>
+        <v>4</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C33" s="4">
-        <v>2894691</v>
+        <v>245350</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="2"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="20">
       <c r="A34" s="2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C34" s="4">
-        <v>1093913</v>
+        <v>21408</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>2</v>
@@ -1640,272 +1617,274 @@
     </row>
     <row r="35" spans="1:5" ht="20">
       <c r="A35" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>5</v>
+        <v>135</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="C35" s="4">
-        <v>245350</v>
+        <v>1546645</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="20">
       <c r="A36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>7</v>
+        <v>43</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="C36" s="4">
-        <v>21408</v>
+        <v>653084</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="20">
       <c r="A37" s="2" t="s">
-        <v>141</v>
+        <v>44</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C37" s="4">
-        <v>1546645</v>
+        <v>2406628</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>69</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5" ht="20">
       <c r="A38" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" s="4">
+        <v>6429</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" s="1" customFormat="1" ht="20">
+      <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C38" s="4">
-        <v>653084</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="20">
-      <c r="A39" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="B39" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C39" s="4">
-        <v>2406628</v>
+        <v>183121</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:5" ht="20">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A40" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C40" s="4">
-        <v>6429</v>
+        <v>1458475</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E40" s="1"/>
+        <v>40</v>
+      </c>
     </row>
     <row r="41" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A41" s="2" t="s">
-        <v>49</v>
+        <v>142</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C41" s="4">
-        <v>183121</v>
+        <v>3109717</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A42" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C42" s="4">
-        <v>1458475</v>
+        <v>2449018</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A43" s="2" t="s">
-        <v>148</v>
+        <v>50</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C43" s="4">
-        <v>3109717</v>
+        <v>2464445</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A44" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="C44" s="4">
-        <v>2449018</v>
+        <v>96797</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A45" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C45" s="4">
-        <v>2464445</v>
+        <v>1703914</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A46" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>3</v>
+        <v>53</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>148</v>
       </c>
       <c r="C46" s="4">
-        <v>96797</v>
+        <v>211474</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A47" s="2" t="s">
-        <v>56</v>
+        <v>149</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C47" s="4">
-        <v>1703914</v>
+        <v>457228</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A48" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C48" s="4">
-        <v>211474</v>
+        <v>3035769</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>43</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A49" s="2" t="s">
-        <v>155</v>
+        <v>55</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C49" s="4">
-        <v>457228</v>
+        <v>559263</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A50" s="2" t="s">
-        <v>58</v>
+        <v>197</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C50" s="4">
-        <v>3035769</v>
+        <v>1487923</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E50" s="2"/>
+        <v>40</v>
+      </c>
     </row>
     <row r="51" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A51" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>158</v>
+        <v>56</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="C51" s="4">
-        <v>559263</v>
+        <v>1378784</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A52" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>160</v>
+        <v>59</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="C52" s="4">
-        <v>1487923</v>
+        <v>405774</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>43</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E52"/>
     </row>
     <row r="53" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A53" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C53" s="4">
-        <v>1378784</v>
+        <v>623218</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>62</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="E53"/>
     </row>
     <row r="54" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A54" s="2" t="s">
@@ -1915,149 +1894,147 @@
         <v>64</v>
       </c>
       <c r="C54" s="4">
-        <v>405774</v>
+        <v>2304606</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E54"/>
+        <v>58</v>
+      </c>
     </row>
     <row r="55" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A55" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>66</v>
+        <v>103</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>154</v>
       </c>
       <c r="C55" s="4">
-        <v>623218</v>
+        <v>247886</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E55"/>
+        <v>65</v>
+      </c>
     </row>
     <row r="56" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A56" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>68</v>
+        <v>155</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>156</v>
       </c>
       <c r="C56" s="4">
-        <v>2304606</v>
+        <v>621686</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A57" s="2" t="s">
-        <v>108</v>
+        <v>66</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C57" s="4">
-        <v>247886</v>
+        <v>383998</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A58" s="2" t="s">
-        <v>162</v>
+        <v>68</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C58" s="4">
-        <v>621686</v>
+        <v>8351</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A59" s="2" t="s">
-        <v>70</v>
+        <v>159</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C59" s="4">
-        <v>383998</v>
+        <v>29472</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A60" s="2" t="s">
-        <v>72</v>
+        <v>161</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C60" s="4">
-        <v>8351</v>
+        <v>13539</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A61" s="2" t="s">
-        <v>166</v>
+        <v>69</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C61" s="4">
-        <v>29472</v>
+        <v>164661</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A62" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>169</v>
+        <v>10</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C62" s="4">
-        <v>13539</v>
+        <v>1056920</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>71</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A63" s="2" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C63" s="4">
-        <v>164661</v>
+        <v>381732</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>71</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A64" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C64" s="4">
-        <v>1056920</v>
+        <v>1820763</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>2</v>
@@ -2065,453 +2042,431 @@
     </row>
     <row r="65" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A65" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>171</v>
+        <v>165</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="C65" s="4">
-        <v>381732</v>
+        <v>615550</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A66" s="2" t="s">
-        <v>8</v>
+        <v>166</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="C66" s="4">
-        <v>1820763</v>
+        <v>12418</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A67" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C67" s="4">
-        <v>615550</v>
+        <v>500</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A68" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>77</v>
+        <v>168</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="C68" s="4">
-        <v>12418</v>
+        <v>161507</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A69" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>78</v>
+        <v>170</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="C69" s="4">
-        <v>500</v>
+        <v>1090113</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A70" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C70" s="4">
-        <v>161507</v>
+        <v>2358</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="71" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A71" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C71" s="4">
-        <v>1090113</v>
+        <v>897106</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="72" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A72" s="2" t="s">
-        <v>179</v>
+        <v>78</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C72" s="4">
-        <v>2358</v>
+        <v>2270044</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="73" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A73" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>182</v>
+        <v>98</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="C73" s="4">
-        <v>897106</v>
+        <v>1825718</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A74" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>183</v>
+        <v>100</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="C74" s="4">
-        <v>2270044</v>
+        <v>672794</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
     </row>
     <row r="75" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A75" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B75" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="C75" s="4">
-        <v>1825718</v>
+        <v>988518</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="76" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A76" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>105</v>
+        <v>177</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>178</v>
       </c>
       <c r="C76" s="4">
-        <v>672794</v>
+        <v>139478</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="77" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A77" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>107</v>
+        <v>79</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>179</v>
       </c>
       <c r="C77" s="4">
-        <v>988518</v>
+        <v>296675</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A78" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C78" s="4">
-        <v>139478</v>
+        <v>195029</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="79" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A79" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C79" s="4">
-        <v>296675</v>
+        <v>45</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="80" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A80" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>188</v>
+        <v>105</v>
       </c>
       <c r="C80" s="4">
-        <v>195029</v>
+        <v>1219340</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="81" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A81" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C81" s="4">
-        <v>45</v>
+        <v>130</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A82" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>110</v>
+        <v>186</v>
       </c>
       <c r="C82" s="4">
-        <v>1219340</v>
+        <v>555561</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A83" s="2" t="s">
-        <v>85</v>
+        <v>187</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C83" s="4">
-        <v>130</v>
+        <v>1599675</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="84" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A84" s="2" t="s">
-        <v>192</v>
+        <v>82</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C84" s="4">
-        <v>555561</v>
+        <v>2300</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A85" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>195</v>
+        <v>34</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C85" s="4">
-        <v>1599675</v>
+        <v>1139312</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>69</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E85" s="2"/>
     </row>
     <row r="86" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A86" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>196</v>
+        <v>36</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="C86" s="4">
-        <v>2300</v>
+        <v>116155</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
     </row>
     <row r="87" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A87" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B87" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="B87" s="5" t="s">
+        <v>190</v>
+      </c>
       <c r="C87" s="4">
-        <v>1139312</v>
+        <v>1008975</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E87" s="2"/>
+        <v>86</v>
+      </c>
     </row>
     <row r="88" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A88" s="2" t="s">
-        <v>39</v>
+        <v>191</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="C88" s="4">
-        <v>116155</v>
+        <v>11864</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="89" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A89" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>197</v>
+        <v>192</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="C89" s="4">
-        <v>1008975</v>
+        <v>1639884</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A90" s="2" t="s">
-        <v>198</v>
+        <v>94</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C90" s="4">
-        <v>11864</v>
+        <v>2043567</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="E90" s="2"/>
     </row>
     <row r="91" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A91" s="2" t="s">
-        <v>199</v>
+        <v>96</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C91" s="4">
-        <v>1639884</v>
+        <v>1767632</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A92" s="2" t="s">
-        <v>98</v>
+        <v>18</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="C92" s="4">
-        <v>2043567</v>
+        <v>1075500</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E92" s="2"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="93" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A93" s="2" t="s">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>101</v>
+        <v>21</v>
       </c>
       <c r="C93" s="4">
-        <v>1767632</v>
+        <v>986023</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
     </row>
     <row r="94" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A94" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C94" s="4">
-        <v>1075500</v>
+        <v>358775</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="1" customFormat="1" ht="20">
-      <c r="A95" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C95" s="4">
-        <v>986023</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" s="1" customFormat="1" ht="20">
-      <c r="A96" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C96" s="4">
-        <v>358775</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>16</v>
-      </c>
+    <row r="95" spans="1:5" s="1" customFormat="1" ht="18">
+      <c r="B95"/>
+    </row>
+    <row r="96" spans="1:5" s="1" customFormat="1" ht="18">
+      <c r="B96"/>
     </row>
     <row r="97" spans="2:2" s="1" customFormat="1" ht="18">
       <c r="B97"/>
@@ -2600,15 +2555,9 @@
     <row r="125" spans="2:2" s="1" customFormat="1" ht="18">
       <c r="B125"/>
     </row>
-    <row r="126" spans="2:2" s="1" customFormat="1" ht="18">
-      <c r="B126"/>
-    </row>
-    <row r="127" spans="2:2" s="1" customFormat="1" ht="18">
-      <c r="B127"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E93">
-    <sortCondition ref="D1:D93"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E91">
+    <sortCondition ref="D1:D91"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Docs] modify excel file
</commit_message>
<xml_diff>
--- a/Projects/App/Resources/onboardingArtist.xlsx
+++ b/Projects/App/Resources/onboardingArtist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choihyowon/Desktop/2023/ADA/Mac/Setlist/Projects/App/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB658EA-6D11-BF42-9030-B6E06DC98FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AE3961-62CE-3F48-8E1E-7469A32A0EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15640" xr2:uid="{DDFC3EF1-0C9B-2449-839F-441E442BC4BA}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="장르별 30명씩" sheetId="9" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'장르별 30명씩'!$A$17:$D$124</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'장르별 30명씩'!$A$17:$D$123</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="197">
   <si>
     <t>카더가든</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -172,10 +172,6 @@
     <t>pH-1</t>
   </si>
   <si>
-    <t>투모로우바이투게더</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>케이팝</t>
   </si>
   <si>
@@ -375,10 +371,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>지코(ZICO)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>be465d46-9615-4722-b828-ea531ff97ea3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -426,21 +418,9 @@
     <t>142b343d-bf5a-428c-a64f-6d1a7566bbe9</t>
   </si>
   <si>
-    <t>PostMalone</t>
-  </si>
-  <si>
-    <t>CharliePuth</t>
-  </si>
-  <si>
-    <t>TaylorSwift</t>
-  </si>
-  <si>
     <t>20244d07-534f-4eff-b4d4-930878889970</t>
   </si>
   <si>
-    <t>SamSmith</t>
-  </si>
-  <si>
     <t>e156615d-3ddd-4491-9584-4b9d971472c4</t>
   </si>
   <si>
@@ -474,9 +454,6 @@
     <t>89e95aa3-bd49-4af3-9c87-0d88b2093bb0</t>
   </si>
   <si>
-    <t>TheKidLAROI</t>
-  </si>
-  <si>
     <t>80609a00-b394-4a49-975b-2db6b543fa97</t>
   </si>
   <si>
@@ -507,18 +484,12 @@
     <t>06bb5fcc-f2b3-428d-b8e7-079060311b6d</t>
   </si>
   <si>
-    <t>PaulKim</t>
-  </si>
-  <si>
     <t>bce172fc-51bb-43f7-9a25-b406a0a581d5</t>
   </si>
   <si>
     <t>8da127cc-c432-418f-b356-ef36210d82ac</t>
   </si>
   <si>
-    <t>RedVelvet</t>
-  </si>
-  <si>
     <t>4f0cb3b7-6c06-4317-ae35-ddf3106a17ee</t>
   </si>
   <si>
@@ -534,9 +505,6 @@
     <t>f1cc066a-6dd1-4b18-ae68-3708472ab4b1</t>
   </si>
   <si>
-    <t>ConanGray</t>
-  </si>
-  <si>
     <t>850a8b03-98a7-4fd3-afbd-5e5520b4ef5f</t>
   </si>
   <si>
@@ -546,9 +514,6 @@
     <t>cc197bad-dc9c-440d-a5b5-d52ba2e14234</t>
   </si>
   <si>
-    <t>ImagineDragons</t>
-  </si>
-  <si>
     <t>012151a8-0f9a-44c9-997f-ebd68b5389f9</t>
   </si>
   <si>
@@ -564,36 +529,12 @@
     <t>dea836e0-66dd-4285-9cab-2272bcda93b8</t>
   </si>
   <si>
-    <t>BillieEilish</t>
-  </si>
-  <si>
-    <t>EdSheeran</t>
-  </si>
-  <si>
-    <t>BrunoMars</t>
-  </si>
-  <si>
-    <t>TroyeSivan</t>
-  </si>
-  <si>
     <t>e5712ceb-c37a-4c49-a11c-ccf4e21852d4</t>
   </si>
   <si>
-    <t>YonezuKenshi</t>
-  </si>
-  <si>
-    <t>09d4a85c-4916-4b4e-bc96-c4cfcf371046</t>
-  </si>
-  <si>
-    <t>TheWeeknd</t>
-  </si>
-  <si>
     <t>c8b03190-306c-4120-bb0b-6f2ebfc06ea9</t>
   </si>
   <si>
-    <t>CentralCee</t>
-  </si>
-  <si>
     <t>b0337af1-8d93-4671-b6c9-ba306bf942bf</t>
   </si>
   <si>
@@ -609,9 +550,6 @@
     <t>e3d5b5ec-101a-4529-9f2d-01dca64cf44e</t>
   </si>
   <si>
-    <t>ShawnMendes</t>
-  </si>
-  <si>
     <t>b7d92248-97e3-4450-8057-6fe06738f735</t>
   </si>
   <si>
@@ -645,9 +583,6 @@
     <t>YoungK</t>
   </si>
   <si>
-    <t>AshIsland</t>
-  </si>
-  <si>
     <t>525f1f1c-03f0-4bc8-8dfd-e7521f87631b</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -669,6 +604,82 @@
   </si>
   <si>
     <t>Sik-k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOMORROW X TOGETHER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Post Malone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Charlie Puth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taylor Swift</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sam Smith</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지코</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Kid LAROI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red Velvet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Paul Kim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Conan Gray</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Imagine Dragons</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Billie Eilish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ed Sheeran</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bruno Mars</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Weeknd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Troye Sivan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Central Cee</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shawn Mendes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ash Island</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1094,10 +1105,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A18E46-C40A-D44C-92D2-00EB00D6AF41}">
-  <dimension ref="A1:E125"/>
+  <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:D26"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="17.25" customHeight="1"/>
@@ -1110,31 +1121,31 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20">
       <c r="A1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C1" s="4">
         <v>70113</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" ht="20">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C2" s="4">
         <v>987404</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -1143,7 +1154,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C3" s="4">
         <v>264991</v>
@@ -1155,76 +1166,76 @@
     </row>
     <row r="4" spans="1:5" ht="20">
       <c r="A4" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C4" s="4">
         <v>994221</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="20">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C5" s="4">
         <v>3239944</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="20">
       <c r="A6" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" s="4">
         <v>11593</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="20">
       <c r="A7" s="6" t="s">
-        <v>39</v>
+        <v>178</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C7" s="4">
         <v>1692196</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" ht="20">
       <c r="A8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C8" s="4">
         <v>961718</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -1245,106 +1256,106 @@
     </row>
     <row r="10" spans="1:5" ht="20">
       <c r="A10" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C10" s="4">
         <v>970192</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="20">
       <c r="A11" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C11" s="4">
         <v>1233909</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="20">
       <c r="A12" s="2" t="s">
-        <v>119</v>
+        <v>179</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" s="4">
         <v>326362</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="20">
       <c r="A13" s="2" t="s">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="C13" s="4">
         <v>250301</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" ht="20">
       <c r="A14" s="2" t="s">
-        <v>121</v>
+        <v>181</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C14" s="4">
         <v>1177</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" ht="20">
       <c r="A15" s="2" t="s">
-        <v>123</v>
+        <v>182</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="4">
         <v>43383</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="20">
       <c r="A16" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="C16" s="4">
         <v>24364</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E16" s="2"/>
     </row>
@@ -1353,7 +1364,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C17" s="4">
         <v>1302105</v>
@@ -1368,7 +1379,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="C18" s="4">
         <v>893747</v>
@@ -1383,7 +1394,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C19" s="4">
         <v>1509383</v>
@@ -1395,52 +1406,52 @@
     </row>
     <row r="20" spans="1:5" ht="20">
       <c r="A20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="C20" s="4">
         <v>39141</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="20">
       <c r="A21" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21" s="4">
         <v>297553</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="20">
       <c r="A22" s="2" t="s">
-        <v>104</v>
+        <v>183</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C22" s="4">
         <v>217593</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" ht="20">
       <c r="A23" s="2" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>33</v>
@@ -1458,7 +1469,7 @@
         <v>28</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C24" s="4">
         <v>318857</v>
@@ -1473,7 +1484,7 @@
         <v>30</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C25" s="4">
         <v>980734</v>
@@ -1485,61 +1496,61 @@
     </row>
     <row r="26" spans="1:5" ht="20">
       <c r="A26" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C26" s="4">
         <v>26507</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" ht="20">
       <c r="A27" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C27" s="4">
         <v>22457</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" ht="20">
       <c r="A28" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C28" s="4">
         <v>338777</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" ht="20">
       <c r="A29" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C29" s="4">
         <v>12024</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E29" s="2"/>
     </row>
@@ -1560,10 +1571,10 @@
     </row>
     <row r="31" spans="1:5" ht="20">
       <c r="A31" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C31" s="4">
         <v>2894691</v>
@@ -1617,135 +1628,135 @@
     </row>
     <row r="35" spans="1:5" ht="20">
       <c r="A35" s="2" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C35" s="4">
         <v>1546645</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="20">
       <c r="A36" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C36" s="4">
         <v>653084</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="20">
       <c r="A37" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C37" s="4">
         <v>2406628</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5" ht="20">
       <c r="A38" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C38" s="4">
         <v>6429</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A39" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C39" s="4">
         <v>183121</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A40" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C40" s="4">
         <v>1458475</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A41" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C41" s="4">
         <v>3109717</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A42" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C42" s="4">
         <v>2449018</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A43" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C43" s="4">
         <v>2464445</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A44" s="2" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>3</v>
@@ -1759,243 +1770,243 @@
     </row>
     <row r="45" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A45" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C45" s="4">
         <v>1703914</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A46" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C46" s="4">
         <v>211474</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A47" s="2" t="s">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C47" s="4">
         <v>457228</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A48" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C48" s="4">
         <v>3035769</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A49" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C49" s="4">
         <v>559263</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A50" s="2" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C50" s="4">
         <v>1487923</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A51" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="C51" s="4">
         <v>1378784</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A52" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="C52" s="4">
         <v>405774</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E52"/>
     </row>
     <row r="53" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A53" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="C53" s="4">
         <v>623218</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E53"/>
     </row>
     <row r="54" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A54" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="C54" s="4">
         <v>2304606</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A55" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C55" s="4">
         <v>247886</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A56" s="2" t="s">
-        <v>155</v>
+        <v>187</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C56" s="4">
         <v>621686</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A57" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C57" s="4">
         <v>383998</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A58" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C58" s="4">
         <v>8351</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A59" s="2" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C59" s="4">
         <v>29472</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A60" s="2" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C60" s="4">
         <v>13539</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A61" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C61" s="4">
         <v>164661</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="1" customFormat="1" ht="20">
@@ -2017,7 +2028,7 @@
         <v>12</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C63" s="4">
         <v>381732</v>
@@ -2042,393 +2053,393 @@
     </row>
     <row r="65" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A65" s="2" t="s">
-        <v>165</v>
+        <v>189</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C65" s="4">
         <v>615550</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A66" s="2" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C66" s="4">
         <v>12418</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A67" s="2" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C67" s="4">
         <v>500</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A68" s="2" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="C68" s="4">
         <v>161507</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A69" s="2" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="C69" s="4">
-        <v>1090113</v>
+        <v>2358</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A70" s="2" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="C70" s="4">
-        <v>2358</v>
+        <v>897106</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="71" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A71" s="2" t="s">
-        <v>174</v>
+        <v>77</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="C71" s="4">
-        <v>897106</v>
+        <v>2270044</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A72" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>176</v>
+        <v>97</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="C72" s="4">
-        <v>2270044</v>
+        <v>1825718</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A73" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C73" s="4">
-        <v>1825718</v>
+        <v>672794</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A74" s="2" t="s">
-        <v>100</v>
+        <v>177</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>101</v>
       </c>
       <c r="C74" s="4">
-        <v>672794</v>
+        <v>988518</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A75" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>102</v>
+        <v>158</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>159</v>
       </c>
       <c r="C75" s="4">
-        <v>988518</v>
+        <v>139478</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
     </row>
     <row r="76" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A76" s="2" t="s">
-        <v>177</v>
+        <v>78</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="C76" s="4">
-        <v>139478</v>
+        <v>296675</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A77" s="2" t="s">
-        <v>79</v>
+        <v>195</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="C77" s="4">
-        <v>296675</v>
+        <v>195029</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="78" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A78" s="2" t="s">
-        <v>180</v>
+        <v>79</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="C78" s="4">
-        <v>195029</v>
+        <v>45</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="79" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A79" s="2" t="s">
-        <v>80</v>
+        <v>163</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>182</v>
+        <v>103</v>
       </c>
       <c r="C79" s="4">
-        <v>45</v>
+        <v>1219340</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="80" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A80" s="2" t="s">
-        <v>183</v>
+        <v>80</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>105</v>
+        <v>164</v>
       </c>
       <c r="C80" s="4">
-        <v>1219340</v>
+        <v>130</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="81" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A81" s="2" t="s">
-        <v>81</v>
+        <v>165</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="C81" s="4">
-        <v>130</v>
+        <v>555561</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A82" s="2" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="C82" s="4">
-        <v>555561</v>
+        <v>1599675</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A83" s="2" t="s">
-        <v>187</v>
+        <v>81</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="C83" s="4">
-        <v>1599675</v>
+        <v>2300</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="84" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A84" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>189</v>
+        <v>34</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C84" s="4">
-        <v>2300</v>
+        <v>1139312</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>65</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E84" s="2"/>
     </row>
     <row r="85" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A85" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C85" s="4">
-        <v>1139312</v>
+        <v>116155</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E85" s="2"/>
     </row>
     <row r="86" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A86" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>170</v>
       </c>
       <c r="C86" s="4">
-        <v>116155</v>
+        <v>1008975</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A87" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>190</v>
+        <v>171</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="C87" s="4">
-        <v>1008975</v>
+        <v>11864</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A88" s="2" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>92</v>
       </c>
       <c r="C88" s="4">
-        <v>11864</v>
+        <v>1639884</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
     </row>
     <row r="89" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A89" s="2" t="s">
-        <v>192</v>
+        <v>93</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C89" s="4">
-        <v>1639884</v>
+        <v>2043567</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>86</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="E89" s="2"/>
     </row>
     <row r="90" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A90" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C90" s="4">
-        <v>2043567</v>
+        <v>1767632</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E90" s="2"/>
+        <v>85</v>
+      </c>
     </row>
     <row r="91" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A91" s="2" t="s">
-        <v>96</v>
+        <v>18</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="C91" s="4">
-        <v>1767632</v>
+        <v>1075500</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A92" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C92" s="4">
-        <v>1075500</v>
+        <v>986023</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>16</v>
@@ -2436,31 +2447,20 @@
     </row>
     <row r="93" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A93" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C93" s="4">
-        <v>986023</v>
+        <v>358775</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="1" customFormat="1" ht="20">
-      <c r="A94" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C94" s="4">
-        <v>358775</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>16</v>
-      </c>
+    <row r="94" spans="1:5" s="1" customFormat="1" ht="18">
+      <c r="B94"/>
     </row>
     <row r="95" spans="1:5" s="1" customFormat="1" ht="18">
       <c r="B95"/>
@@ -2552,12 +2552,9 @@
     <row r="124" spans="2:2" s="1" customFormat="1" ht="18">
       <c r="B124"/>
     </row>
-    <row r="125" spans="2:2" s="1" customFormat="1" ht="18">
-      <c r="B125"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E91">
-    <sortCondition ref="D1:D91"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E90">
+    <sortCondition ref="D1:D90"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Feat]#128 - complete searchArtist
</commit_message>
<xml_diff>
--- a/Projects/App/Resources/onboardingArtist.xlsx
+++ b/Projects/App/Resources/onboardingArtist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choihyowon/Desktop/2023/ADA/Mac/Setlist/Projects/App/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AE3961-62CE-3F48-8E1E-7469A32A0EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB9BEE1-07DC-444B-8B27-C32BB14FD731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15640" xr2:uid="{DDFC3EF1-0C9B-2449-839F-441E442BC4BA}"/>
   </bookViews>
@@ -436,9 +436,6 @@
     <t>a697464c-69b1-4bbc-88cc-570c025a25e5</t>
   </si>
   <si>
-    <t>ArianaGrande</t>
-  </si>
-  <si>
     <t>HarryStyles</t>
   </si>
   <si>
@@ -680,6 +677,10 @@
   </si>
   <si>
     <t>Ash Island</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ariana Grande</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1107,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A18E46-C40A-D44C-92D2-00EB00D6AF41}">
   <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="17.25" customHeight="1"/>
@@ -1211,7 +1212,7 @@
     </row>
     <row r="7" spans="1:5" ht="20">
       <c r="A7" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>111</v>
@@ -1286,7 +1287,7 @@
     </row>
     <row r="12" spans="1:5" ht="20">
       <c r="A12" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>69</v>
@@ -1301,10 +1302,10 @@
     </row>
     <row r="13" spans="1:5" ht="20">
       <c r="A13" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C13" s="4">
         <v>250301</v>
@@ -1316,7 +1317,7 @@
     </row>
     <row r="14" spans="1:5" ht="20">
       <c r="A14" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>117</v>
@@ -1331,7 +1332,7 @@
     </row>
     <row r="15" spans="1:5" ht="20">
       <c r="A15" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>70</v>
@@ -1349,7 +1350,7 @@
         <v>84</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C16" s="4">
         <v>24364</v>
@@ -1379,7 +1380,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C18" s="4">
         <v>893747</v>
@@ -1436,7 +1437,7 @@
     </row>
     <row r="22" spans="1:5" ht="20">
       <c r="A22" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>90</v>
@@ -1451,7 +1452,7 @@
     </row>
     <row r="23" spans="1:5" ht="20">
       <c r="A23" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>33</v>
@@ -1496,7 +1497,7 @@
     </row>
     <row r="26" spans="1:5" ht="20">
       <c r="A26" s="2" t="s">
-        <v>123</v>
+        <v>196</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>74</v>
@@ -1511,7 +1512,7 @@
     </row>
     <row r="27" spans="1:5" ht="20">
       <c r="A27" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>75</v>
@@ -1529,7 +1530,7 @@
         <v>76</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C28" s="4">
         <v>338777</v>
@@ -1544,7 +1545,7 @@
         <v>82</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C29" s="4">
         <v>12024</v>
@@ -1571,10 +1572,10 @@
     </row>
     <row r="31" spans="1:5" ht="20">
       <c r="A31" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>127</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>128</v>
       </c>
       <c r="C31" s="4">
         <v>2894691</v>
@@ -1628,10 +1629,10 @@
     </row>
     <row r="35" spans="1:5" ht="20">
       <c r="A35" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C35" s="4">
         <v>1546645</v>
@@ -1645,7 +1646,7 @@
         <v>42</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C36" s="4">
         <v>653084</v>
@@ -1659,7 +1660,7 @@
         <v>43</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C37" s="4">
         <v>2406628</v>
@@ -1674,7 +1675,7 @@
         <v>44</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C38" s="4">
         <v>6429</v>
@@ -1689,7 +1690,7 @@
         <v>45</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C39" s="4">
         <v>183121</v>
@@ -1703,7 +1704,7 @@
         <v>47</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C40" s="4">
         <v>1458475</v>
@@ -1714,10 +1715,10 @@
     </row>
     <row r="41" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A41" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>136</v>
       </c>
       <c r="C41" s="4">
         <v>3109717</v>
@@ -1731,7 +1732,7 @@
         <v>48</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C42" s="4">
         <v>2449018</v>
@@ -1745,7 +1746,7 @@
         <v>49</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C43" s="4">
         <v>2464445</v>
@@ -1756,7 +1757,7 @@
     </row>
     <row r="44" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A44" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>3</v>
@@ -1773,7 +1774,7 @@
         <v>51</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C45" s="4">
         <v>1703914</v>
@@ -1787,7 +1788,7 @@
         <v>52</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C46" s="4">
         <v>211474</v>
@@ -1798,10 +1799,10 @@
     </row>
     <row r="47" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A47" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C47" s="4">
         <v>457228</v>
@@ -1815,7 +1816,7 @@
         <v>53</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C48" s="4">
         <v>3035769</v>
@@ -1830,7 +1831,7 @@
         <v>54</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C49" s="4">
         <v>559263</v>
@@ -1841,10 +1842,10 @@
     </row>
     <row r="50" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A50" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C50" s="4">
         <v>1487923</v>
@@ -1916,7 +1917,7 @@
         <v>102</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C55" s="4">
         <v>247886</v>
@@ -1927,10 +1928,10 @@
     </row>
     <row r="56" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A56" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C56" s="4">
         <v>621686</v>
@@ -1944,7 +1945,7 @@
         <v>65</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C57" s="4">
         <v>383998</v>
@@ -1958,7 +1959,7 @@
         <v>67</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C58" s="4">
         <v>8351</v>
@@ -1969,10 +1970,10 @@
     </row>
     <row r="59" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A59" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C59" s="4">
         <v>29472</v>
@@ -1983,10 +1984,10 @@
     </row>
     <row r="60" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A60" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>151</v>
       </c>
       <c r="C60" s="4">
         <v>13539</v>
@@ -2000,7 +2001,7 @@
         <v>68</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C61" s="4">
         <v>164661</v>
@@ -2028,7 +2029,7 @@
         <v>12</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C63" s="4">
         <v>381732</v>
@@ -2053,7 +2054,7 @@
     </row>
     <row r="65" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A65" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>71</v>
@@ -2067,7 +2068,7 @@
     </row>
     <row r="66" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A66" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>72</v>
@@ -2081,7 +2082,7 @@
     </row>
     <row r="67" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A67" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>73</v>
@@ -2095,10 +2096,10 @@
     </row>
     <row r="68" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A68" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C68" s="4">
         <v>161507</v>
@@ -2109,10 +2110,10 @@
     </row>
     <row r="69" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A69" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C69" s="4">
         <v>2358</v>
@@ -2123,10 +2124,10 @@
     </row>
     <row r="70" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A70" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C70" s="4">
         <v>897106</v>
@@ -2140,7 +2141,7 @@
         <v>77</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C71" s="4">
         <v>2270044</v>
@@ -2179,7 +2180,7 @@
     </row>
     <row r="74" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A74" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>101</v>
@@ -2193,10 +2194,10 @@
     </row>
     <row r="75" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A75" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>159</v>
       </c>
       <c r="C75" s="4">
         <v>139478</v>
@@ -2210,7 +2211,7 @@
         <v>78</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C76" s="4">
         <v>296675</v>
@@ -2221,10 +2222,10 @@
     </row>
     <row r="77" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A77" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C77" s="4">
         <v>195029</v>
@@ -2238,7 +2239,7 @@
         <v>79</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C78" s="4">
         <v>45</v>
@@ -2249,7 +2250,7 @@
     </row>
     <row r="79" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A79" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>103</v>
@@ -2266,7 +2267,7 @@
         <v>80</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C80" s="4">
         <v>130</v>
@@ -2277,10 +2278,10 @@
     </row>
     <row r="81" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A81" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B81" s="5" t="s">
         <v>165</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>166</v>
       </c>
       <c r="C81" s="4">
         <v>555561</v>
@@ -2291,10 +2292,10 @@
     </row>
     <row r="82" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A82" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B82" s="5" t="s">
         <v>167</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>168</v>
       </c>
       <c r="C82" s="4">
         <v>1599675</v>
@@ -2308,7 +2309,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C83" s="4">
         <v>2300</v>
@@ -2351,7 +2352,7 @@
         <v>38</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C86" s="4">
         <v>1008975</v>
@@ -2362,7 +2363,7 @@
     </row>
     <row r="87" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A87" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>91</v>
@@ -2376,7 +2377,7 @@
     </row>
     <row r="88" spans="1:5" s="1" customFormat="1" ht="20">
       <c r="A88" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>92</v>

</xml_diff>